<commit_message>
Finished ew.issue.19180323; moved to tei_final 4/4/2017
</commit_message>
<xml_diff>
--- a/spreadsheet/EW.xlsx
+++ b/spreadsheet/EW.xlsx
@@ -5,7 +5,7 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\Projects\Every Week\Administration\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eridwi\Documents\GitHub\data_everyweek\spreadsheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1426" uniqueCount="284">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1427" uniqueCount="284">
   <si>
     <t>File Name</t>
   </si>
@@ -1356,7 +1356,7 @@
   <dimension ref="A1:Q168"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A143" zoomScaleNormal="100" zoomScalePageLayoutView="159" workbookViewId="0">
-      <selection activeCell="I154" sqref="I154"/>
+      <selection activeCell="J152" sqref="J152"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -7611,8 +7611,11 @@
       <c r="G153" t="s">
         <v>70</v>
       </c>
-      <c r="H153" s="20" t="s">
-        <v>191</v>
+      <c r="H153" s="9" t="s">
+        <v>282</v>
+      </c>
+      <c r="I153" t="s">
+        <v>6</v>
       </c>
       <c r="P153" t="s">
         <v>6</v>

</xml_diff>

<commit_message>
Finished ew.issue.19180406 4/18/2017, moved to tei_final; updated spreadsheet
</commit_message>
<xml_diff>
--- a/spreadsheet/EW.xlsx
+++ b/spreadsheet/EW.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1429" uniqueCount="284">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1430" uniqueCount="284">
   <si>
     <t>File Name</t>
   </si>
@@ -1356,7 +1356,7 @@
   <dimension ref="A1:Q168"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A145" zoomScaleNormal="100" zoomScalePageLayoutView="159" workbookViewId="0">
-      <selection activeCell="I155" sqref="I155"/>
+      <selection activeCell="K153" sqref="K153"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -7710,8 +7710,11 @@
       <c r="G156" t="s">
         <v>70</v>
       </c>
-      <c r="H156" s="20" t="s">
-        <v>190</v>
+      <c r="H156" s="9" t="s">
+        <v>281</v>
+      </c>
+      <c r="I156" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="157" spans="1:16" s="21" customFormat="1">

</xml_diff>

<commit_message>
Finished ew.issue.19180420, moved to tei_final; updated spreadsheet
</commit_message>
<xml_diff>
--- a/spreadsheet/EW.xlsx
+++ b/spreadsheet/EW.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1430" uniqueCount="284">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1431" uniqueCount="284">
   <si>
     <t>File Name</t>
   </si>
@@ -1356,7 +1356,7 @@
   <dimension ref="A1:Q168"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A145" zoomScaleNormal="100" zoomScalePageLayoutView="159" workbookViewId="0">
-      <selection activeCell="K153" sqref="K153"/>
+      <selection activeCell="J160" sqref="J160"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -7774,8 +7774,11 @@
       <c r="G158" t="s">
         <v>70</v>
       </c>
-      <c r="H158" s="20" t="s">
-        <v>190</v>
+      <c r="H158" s="9" t="s">
+        <v>281</v>
+      </c>
+      <c r="I158" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="159" spans="1:16">

</xml_diff>

<commit_message>
Finished ew.issue.19180427 4/28/2017, moved to tei_final; updated spreadsheet
</commit_message>
<xml_diff>
--- a/spreadsheet/EW.xlsx
+++ b/spreadsheet/EW.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1431" uniqueCount="284">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1432" uniqueCount="284">
   <si>
     <t>File Name</t>
   </si>
@@ -1356,7 +1356,7 @@
   <dimension ref="A1:Q168"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A145" zoomScaleNormal="100" zoomScalePageLayoutView="159" workbookViewId="0">
-      <selection activeCell="J160" sqref="J160"/>
+      <selection activeCell="J161" sqref="J161"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -7804,8 +7804,11 @@
       <c r="G159" t="s">
         <v>70</v>
       </c>
-      <c r="H159" s="20" t="s">
-        <v>190</v>
+      <c r="H159" s="9" t="s">
+        <v>281</v>
+      </c>
+      <c r="I159" t="s">
+        <v>6</v>
       </c>
       <c r="P159" t="s">
         <v>6</v>

</xml_diff>

<commit_message>
Finished ew.issue.19180504 on 5/1/2017, moved to tei_final; updated spreadsheet
</commit_message>
<xml_diff>
--- a/spreadsheet/EW.xlsx
+++ b/spreadsheet/EW.xlsx
@@ -940,7 +940,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -956,12 +956,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="3" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -990,7 +984,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1034,12 +1028,11 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="16" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="16" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="16" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
@@ -1358,8 +1351,8 @@
   </sheetPr>
   <dimension ref="A1:Q168"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A127" zoomScaleNormal="100" zoomScalePageLayoutView="159" workbookViewId="0">
-      <selection activeCell="L133" sqref="L133"/>
+    <sheetView tabSelected="1" topLeftCell="A145" zoomScaleNormal="100" zoomScalePageLayoutView="159" workbookViewId="0">
+      <selection activeCell="J165" sqref="J165"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -7107,7 +7100,7 @@
         <v>2</v>
       </c>
       <c r="F138" s="14"/>
-      <c r="G138" s="25" t="s">
+      <c r="G138" s="24" t="s">
         <v>70</v>
       </c>
       <c r="H138" s="16" t="s">
@@ -7720,39 +7713,39 @@
         <v>6</v>
       </c>
     </row>
-    <row r="157" spans="1:16" s="21" customFormat="1">
-      <c r="A157" s="21" t="s">
+    <row r="157" spans="1:16" s="20" customFormat="1">
+      <c r="A157" s="20" t="s">
         <v>175</v>
       </c>
-      <c r="B157" s="21" t="s">
-        <v>11</v>
-      </c>
-      <c r="C157" s="22">
-        <v>24</v>
-      </c>
-      <c r="D157" s="22">
-        <v>24</v>
-      </c>
-      <c r="E157" s="22">
+      <c r="B157" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="C157" s="21">
+        <v>24</v>
+      </c>
+      <c r="D157" s="21">
+        <v>24</v>
+      </c>
+      <c r="E157" s="21">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F157" s="22">
-        <v>0</v>
-      </c>
-      <c r="G157" s="23" t="s">
-        <v>70</v>
-      </c>
-      <c r="H157" s="21" t="s">
+      <c r="F157" s="21">
+        <v>0</v>
+      </c>
+      <c r="G157" s="22" t="s">
+        <v>70</v>
+      </c>
+      <c r="H157" s="20" t="s">
         <v>190</v>
       </c>
-      <c r="L157" s="24" t="s">
+      <c r="L157" s="23" t="s">
         <v>284</v>
       </c>
-      <c r="M157" s="21" t="s">
-        <v>105</v>
-      </c>
-      <c r="N157" s="21" t="s">
+      <c r="M157" s="20" t="s">
+        <v>105</v>
+      </c>
+      <c r="N157" s="20" t="s">
         <v>184</v>
       </c>
     </row>
@@ -7843,7 +7836,7 @@
         <v>70</v>
       </c>
       <c r="H160" s="16" t="s">
-        <v>191</v>
+        <v>281</v>
       </c>
       <c r="I160" s="16" t="s">
         <v>258</v>
@@ -7856,39 +7849,40 @@
         <v>187</v>
       </c>
     </row>
-    <row r="161" spans="1:16">
-      <c r="A161" t="s">
+    <row r="161" spans="1:16" s="16" customFormat="1">
+      <c r="A161" s="16" t="s">
         <v>177</v>
       </c>
-      <c r="B161" t="s">
-        <v>11</v>
-      </c>
-      <c r="C161" s="1">
-        <v>24</v>
-      </c>
-      <c r="D161" s="1">
-        <v>20</v>
-      </c>
-      <c r="E161" s="1">
+      <c r="B161" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="C161" s="14">
+        <v>24</v>
+      </c>
+      <c r="D161" s="14">
+        <v>20</v>
+      </c>
+      <c r="E161" s="14">
         <f t="shared" si="2"/>
         <v>4</v>
       </c>
-      <c r="F161" s="1">
-        <v>0</v>
-      </c>
-      <c r="G161" t="s">
-        <v>70</v>
-      </c>
-      <c r="H161" s="20" t="s">
+      <c r="F161" s="14">
+        <v>0</v>
+      </c>
+      <c r="G161" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="H161" s="16" t="s">
         <v>191</v>
       </c>
-      <c r="I161" t="s">
+      <c r="I161" s="16" t="s">
         <v>258</v>
       </c>
-      <c r="M161" t="s">
-        <v>105</v>
-      </c>
-      <c r="N161" t="s">
+      <c r="L161" s="17"/>
+      <c r="M161" s="16" t="s">
+        <v>105</v>
+      </c>
+      <c r="N161" s="16" t="s">
         <v>187</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Finished ew.issue.19180511 on 5/2/2017; moved to tei_final; updated spreadsheet
</commit_message>
<xml_diff>
--- a/spreadsheet/EW.xlsx
+++ b/spreadsheet/EW.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1435" uniqueCount="285">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1435" uniqueCount="284">
   <si>
     <t>File Name</t>
   </si>
@@ -602,9 +602,6 @@
   </si>
   <si>
     <t>KH/</t>
-  </si>
-  <si>
-    <t>KH</t>
   </si>
   <si>
     <t>CHO/LW</t>
@@ -1351,7 +1348,7 @@
   </sheetPr>
   <dimension ref="A1:Q168"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A145" zoomScaleNormal="100" zoomScalePageLayoutView="159" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A136" zoomScaleNormal="100" zoomScalePageLayoutView="159" workbookViewId="0">
       <selection activeCell="J165" sqref="J165"/>
     </sheetView>
   </sheetViews>
@@ -1379,19 +1376,19 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>259</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="D1" s="5" t="s">
         <v>260</v>
       </c>
-      <c r="D1" s="5" t="s">
-        <v>261</v>
-      </c>
       <c r="E1" s="5" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>1</v>
@@ -1400,13 +1397,13 @@
         <v>2</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="J1" s="2" t="s">
         <v>3</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="L1" s="5" t="s">
         <v>58</v>
@@ -1418,13 +1415,13 @@
         <v>183</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="P1" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="Q1" s="1" t="s">
         <v>278</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>279</v>
       </c>
     </row>
     <row r="2" spans="1:17" s="3" customFormat="1">
@@ -1484,19 +1481,19 @@
         <v>71</v>
       </c>
       <c r="H3" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="I3" s="11" t="s">
         <v>6</v>
       </c>
       <c r="J3" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="K3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="L3" s="7" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="M3" t="s">
         <v>105</v>
@@ -1505,7 +1502,7 @@
         <v>187</v>
       </c>
       <c r="O3" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="4" spans="1:17" ht="75">
@@ -1531,19 +1528,19 @@
         <v>71</v>
       </c>
       <c r="H4" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="I4" s="9" t="s">
         <v>6</v>
       </c>
       <c r="J4" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="K4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="L4" s="7" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="M4" t="s">
         <v>105</v>
@@ -1552,7 +1549,7 @@
         <v>187</v>
       </c>
       <c r="O4" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="5" spans="1:17" ht="60">
@@ -1578,19 +1575,19 @@
         <v>71</v>
       </c>
       <c r="H5" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="I5" s="9" t="s">
         <v>6</v>
       </c>
       <c r="J5" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="K5" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="L5" s="7" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="M5" t="s">
         <v>105</v>
@@ -1599,7 +1596,7 @@
         <v>187</v>
       </c>
       <c r="O5" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="6" spans="1:17">
@@ -1625,16 +1622,16 @@
         <v>185</v>
       </c>
       <c r="H6" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="I6" t="s">
         <v>6</v>
       </c>
       <c r="J6" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="K6" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="M6" t="s">
         <v>105</v>
@@ -1643,7 +1640,7 @@
         <v>187</v>
       </c>
       <c r="O6" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="7" spans="1:17">
@@ -1669,16 +1666,16 @@
         <v>186</v>
       </c>
       <c r="H7" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="I7" t="s">
         <v>6</v>
       </c>
       <c r="J7" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="K7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="M7" t="s">
         <v>105</v>
@@ -1687,7 +1684,7 @@
         <v>187</v>
       </c>
       <c r="O7" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="8" spans="1:17">
@@ -1713,16 +1710,16 @@
         <v>185</v>
       </c>
       <c r="H8" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="I8" t="s">
         <v>6</v>
       </c>
       <c r="J8" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="K8" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="M8" t="s">
         <v>105</v>
@@ -1731,7 +1728,7 @@
         <v>187</v>
       </c>
       <c r="O8" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="9" spans="1:17">
@@ -1757,16 +1754,16 @@
         <v>185</v>
       </c>
       <c r="H9" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="I9" t="s">
         <v>6</v>
       </c>
       <c r="J9" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="K9" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="M9" t="s">
         <v>105</v>
@@ -1775,7 +1772,7 @@
         <v>187</v>
       </c>
       <c r="O9" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="10" spans="1:17">
@@ -1801,19 +1798,19 @@
         <v>185</v>
       </c>
       <c r="H10" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="I10" t="s">
         <v>6</v>
       </c>
       <c r="J10" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="K10" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="L10" s="7" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="M10" t="s">
         <v>105</v>
@@ -1822,7 +1819,7 @@
         <v>187</v>
       </c>
       <c r="O10" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="11" spans="1:17">
@@ -1848,16 +1845,16 @@
         <v>185</v>
       </c>
       <c r="H11" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="I11" t="s">
         <v>6</v>
       </c>
       <c r="J11" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="K11" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="M11" t="s">
         <v>105</v>
@@ -1866,7 +1863,7 @@
         <v>187</v>
       </c>
       <c r="O11" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="12" spans="1:17" ht="30">
@@ -1892,19 +1889,19 @@
         <v>188</v>
       </c>
       <c r="H12" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="I12" t="s">
         <v>6</v>
       </c>
       <c r="J12" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="K12" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="L12" s="7" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="M12" t="s">
         <v>105</v>
@@ -1913,7 +1910,7 @@
         <v>187</v>
       </c>
       <c r="O12" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="13" spans="1:17" ht="45">
@@ -1939,19 +1936,19 @@
         <v>188</v>
       </c>
       <c r="H13" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="I13" s="9" t="s">
         <v>6</v>
       </c>
       <c r="J13" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="K13" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="L13" s="7" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="M13" t="s">
         <v>105</v>
@@ -1960,7 +1957,7 @@
         <v>187</v>
       </c>
       <c r="O13" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="14" spans="1:17">
@@ -1986,16 +1983,16 @@
         <v>188</v>
       </c>
       <c r="H14" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="I14" t="s">
         <v>6</v>
       </c>
       <c r="J14" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="K14" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="M14" t="s">
         <v>105</v>
@@ -2004,7 +2001,7 @@
         <v>187</v>
       </c>
       <c r="O14" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="15" spans="1:17">
@@ -2030,19 +2027,19 @@
         <v>188</v>
       </c>
       <c r="H15" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I15" t="s">
         <v>6</v>
       </c>
       <c r="J15" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="K15" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="L15" s="7" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="M15" t="s">
         <v>105</v>
@@ -2051,7 +2048,7 @@
         <v>187</v>
       </c>
       <c r="O15" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="16" spans="1:17">
@@ -2077,19 +2074,19 @@
         <v>188</v>
       </c>
       <c r="H16" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I16" t="s">
         <v>6</v>
       </c>
       <c r="J16" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="K16" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="L16" s="7" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="M16" t="s">
         <v>105</v>
@@ -2098,7 +2095,7 @@
         <v>187</v>
       </c>
       <c r="O16" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="17" spans="1:16">
@@ -2124,16 +2121,16 @@
         <v>188</v>
       </c>
       <c r="H17" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I17" t="s">
         <v>6</v>
       </c>
       <c r="J17" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="K17" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="M17" t="s">
         <v>105</v>
@@ -2142,7 +2139,7 @@
         <v>187</v>
       </c>
       <c r="O17" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="18" spans="1:16">
@@ -2178,10 +2175,10 @@
         <v>73</v>
       </c>
       <c r="K18" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="L18" s="7" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="19" spans="1:16">
@@ -2207,16 +2204,16 @@
         <v>188</v>
       </c>
       <c r="H19" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I19" t="s">
         <v>6</v>
       </c>
       <c r="J19" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="K19" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="M19" t="s">
         <v>105</v>
@@ -2225,7 +2222,7 @@
         <v>187</v>
       </c>
       <c r="O19" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="20" spans="1:16">
@@ -2251,19 +2248,19 @@
         <v>188</v>
       </c>
       <c r="H20" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I20" t="s">
         <v>6</v>
       </c>
       <c r="J20" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="K20" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="L20" s="7" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="M20" t="s">
         <v>105</v>
@@ -2272,7 +2269,7 @@
         <v>187</v>
       </c>
       <c r="O20" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="21" spans="1:16">
@@ -2298,16 +2295,16 @@
         <v>188</v>
       </c>
       <c r="H21" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I21" t="s">
         <v>6</v>
       </c>
       <c r="J21" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="K21" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="M21" t="s">
         <v>105</v>
@@ -2316,7 +2313,7 @@
         <v>187</v>
       </c>
       <c r="O21" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="22" spans="1:16">
@@ -2342,16 +2339,16 @@
         <v>188</v>
       </c>
       <c r="H22" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I22" t="s">
         <v>6</v>
       </c>
       <c r="J22" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="K22" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="M22" t="s">
         <v>105</v>
@@ -2360,7 +2357,7 @@
         <v>187</v>
       </c>
       <c r="O22" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="23" spans="1:16">
@@ -2386,16 +2383,16 @@
         <v>188</v>
       </c>
       <c r="H23" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I23" t="s">
         <v>6</v>
       </c>
       <c r="J23" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="K23" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="M23" t="s">
         <v>105</v>
@@ -2404,7 +2401,7 @@
         <v>187</v>
       </c>
       <c r="O23" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="24" spans="1:16">
@@ -2440,7 +2437,7 @@
         <v>73</v>
       </c>
       <c r="K24" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="25" spans="1:16">
@@ -2466,16 +2463,16 @@
         <v>188</v>
       </c>
       <c r="H25" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I25" t="s">
         <v>6</v>
       </c>
       <c r="J25" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="K25" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="M25" t="s">
         <v>105</v>
@@ -2484,7 +2481,7 @@
         <v>187</v>
       </c>
       <c r="O25" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="26" spans="1:16">
@@ -2510,16 +2507,16 @@
         <v>188</v>
       </c>
       <c r="H26" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I26" t="s">
         <v>6</v>
       </c>
       <c r="J26" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="K26" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="M26" t="s">
         <v>105</v>
@@ -2528,7 +2525,7 @@
         <v>187</v>
       </c>
       <c r="O26" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="27" spans="1:16">
@@ -2555,16 +2552,16 @@
         <v>188</v>
       </c>
       <c r="H27" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I27" t="s">
         <v>6</v>
       </c>
       <c r="J27" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="K27" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="M27" t="s">
         <v>105</v>
@@ -2596,13 +2593,13 @@
         <v>188</v>
       </c>
       <c r="H28" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I28" t="s">
         <v>6</v>
       </c>
       <c r="J28" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="M28" t="s">
         <v>105</v>
@@ -2611,7 +2608,7 @@
         <v>187</v>
       </c>
       <c r="O28" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="29" spans="1:16" ht="30">
@@ -2637,19 +2634,19 @@
         <v>188</v>
       </c>
       <c r="H29" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I29" t="s">
         <v>6</v>
       </c>
       <c r="J29" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="K29" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="L29" s="7" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="M29" t="s">
         <v>105</v>
@@ -2658,7 +2655,7 @@
         <v>187</v>
       </c>
       <c r="O29" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="30" spans="1:16" ht="45">
@@ -2684,19 +2681,19 @@
         <v>188</v>
       </c>
       <c r="H30" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I30" t="s">
         <v>6</v>
       </c>
       <c r="J30" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="K30" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="L30" s="7" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="M30" t="s">
         <v>105</v>
@@ -2705,7 +2702,7 @@
         <v>187</v>
       </c>
       <c r="P30" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="31" spans="1:16" ht="30">
@@ -2731,19 +2728,19 @@
         <v>188</v>
       </c>
       <c r="H31" s="16" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I31" s="18" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="J31" s="16" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="K31" s="16" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="L31" s="17" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="M31" s="16" t="s">
         <v>105</v>
@@ -2752,7 +2749,7 @@
         <v>187</v>
       </c>
       <c r="O31" s="16" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="32" spans="1:16">
@@ -2778,19 +2775,19 @@
         <v>188</v>
       </c>
       <c r="H32" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I32" t="s">
         <v>6</v>
       </c>
       <c r="J32" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="K32" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="L32" s="7" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="M32" t="s">
         <v>105</v>
@@ -2799,7 +2796,7 @@
         <v>187</v>
       </c>
       <c r="O32" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="33" spans="1:16">
@@ -2825,16 +2822,16 @@
         <v>188</v>
       </c>
       <c r="H33" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I33" t="s">
         <v>6</v>
       </c>
       <c r="J33" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="K33" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="M33" t="s">
         <v>105</v>
@@ -2843,7 +2840,7 @@
         <v>187</v>
       </c>
       <c r="P33" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="34" spans="1:16">
@@ -2869,16 +2866,16 @@
         <v>188</v>
       </c>
       <c r="H34" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I34" t="s">
         <v>6</v>
       </c>
       <c r="J34" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="K34" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="M34" t="s">
         <v>105</v>
@@ -2887,7 +2884,7 @@
         <v>187</v>
       </c>
       <c r="O34" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="35" spans="1:16">
@@ -2913,19 +2910,19 @@
         <v>188</v>
       </c>
       <c r="H35" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I35" t="s">
         <v>6</v>
       </c>
       <c r="J35" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="K35" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="L35" s="7" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="M35" t="s">
         <v>105</v>
@@ -2934,7 +2931,7 @@
         <v>187</v>
       </c>
       <c r="O35" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="36" spans="1:16">
@@ -2960,16 +2957,16 @@
         <v>188</v>
       </c>
       <c r="H36" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I36" t="s">
         <v>6</v>
       </c>
       <c r="J36" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="K36" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="M36" t="s">
         <v>105</v>
@@ -2978,7 +2975,7 @@
         <v>187</v>
       </c>
       <c r="O36" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="37" spans="1:16">
@@ -3004,20 +3001,20 @@
         <v>188</v>
       </c>
       <c r="H37" t="s">
+        <v>192</v>
+      </c>
+      <c r="I37" t="s">
+        <v>6</v>
+      </c>
+      <c r="J37" t="s">
+        <v>255</v>
+      </c>
+      <c r="K37" t="s">
+        <v>202</v>
+      </c>
+      <c r="L37" s="7" t="s">
         <v>193</v>
       </c>
-      <c r="I37" t="s">
-        <v>6</v>
-      </c>
-      <c r="J37" t="s">
-        <v>256</v>
-      </c>
-      <c r="K37" t="s">
-        <v>203</v>
-      </c>
-      <c r="L37" s="7" t="s">
-        <v>194</v>
-      </c>
       <c r="M37" t="s">
         <v>105</v>
       </c>
@@ -3025,7 +3022,7 @@
         <v>187</v>
       </c>
       <c r="O37" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="38" spans="1:16" s="16" customFormat="1" ht="30">
@@ -3051,19 +3048,19 @@
         <v>188</v>
       </c>
       <c r="H38" s="16" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I38" s="16" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="J38" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="K38" s="16" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="L38" s="17" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="M38" s="16" t="s">
         <v>105</v>
@@ -3072,7 +3069,7 @@
         <v>187</v>
       </c>
       <c r="O38" s="16" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="39" spans="1:16">
@@ -3098,19 +3095,19 @@
         <v>188</v>
       </c>
       <c r="H39" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I39" t="s">
         <v>6</v>
       </c>
       <c r="J39" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="K39" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="L39" s="7" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="M39" t="s">
         <v>105</v>
@@ -3119,7 +3116,7 @@
         <v>187</v>
       </c>
       <c r="O39" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="40" spans="1:16">
@@ -3145,19 +3142,19 @@
         <v>188</v>
       </c>
       <c r="H40" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I40" t="s">
         <v>6</v>
       </c>
       <c r="J40" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="K40" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="L40" s="7" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="M40" t="s">
         <v>105</v>
@@ -3166,7 +3163,7 @@
         <v>187</v>
       </c>
       <c r="O40" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="41" spans="1:16">
@@ -3192,19 +3189,19 @@
         <v>188</v>
       </c>
       <c r="H41" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I41" t="s">
         <v>6</v>
       </c>
       <c r="J41" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="K41" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="L41" s="7" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="M41" t="s">
         <v>105</v>
@@ -3213,7 +3210,7 @@
         <v>187</v>
       </c>
       <c r="O41" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="42" spans="1:16">
@@ -3239,19 +3236,19 @@
         <v>188</v>
       </c>
       <c r="H42" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I42" t="s">
         <v>6</v>
       </c>
       <c r="J42" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="K42" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="L42" s="7" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="M42" t="s">
         <v>105</v>
@@ -3260,7 +3257,7 @@
         <v>187</v>
       </c>
       <c r="O42" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="43" spans="1:16">
@@ -3286,19 +3283,19 @@
         <v>188</v>
       </c>
       <c r="H43" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I43" t="s">
         <v>6</v>
       </c>
       <c r="J43" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="K43" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="L43" s="15" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="M43" t="s">
         <v>105</v>
@@ -3307,7 +3304,7 @@
         <v>187</v>
       </c>
       <c r="O43" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="44" spans="1:16">
@@ -3333,16 +3330,16 @@
         <v>188</v>
       </c>
       <c r="H44" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I44" t="s">
         <v>6</v>
       </c>
       <c r="J44" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="K44" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="M44" t="s">
         <v>105</v>
@@ -3351,7 +3348,7 @@
         <v>187</v>
       </c>
       <c r="O44" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="45" spans="1:16">
@@ -3377,16 +3374,16 @@
         <v>188</v>
       </c>
       <c r="H45" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I45" t="s">
         <v>6</v>
       </c>
       <c r="J45" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="K45" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="M45" t="s">
         <v>105</v>
@@ -3395,7 +3392,7 @@
         <v>187</v>
       </c>
       <c r="O45" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="46" spans="1:16">
@@ -3421,16 +3418,16 @@
         <v>188</v>
       </c>
       <c r="H46" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I46" t="s">
         <v>6</v>
       </c>
       <c r="J46" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="K46" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="M46" t="s">
         <v>105</v>
@@ -3439,7 +3436,7 @@
         <v>187</v>
       </c>
       <c r="O46" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="47" spans="1:16">
@@ -3465,16 +3462,16 @@
         <v>188</v>
       </c>
       <c r="H47" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I47" t="s">
         <v>6</v>
       </c>
       <c r="J47" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="K47" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="M47" t="s">
         <v>105</v>
@@ -3483,7 +3480,7 @@
         <v>187</v>
       </c>
       <c r="O47" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="48" spans="1:16">
@@ -3509,16 +3506,16 @@
         <v>188</v>
       </c>
       <c r="H48" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I48" t="s">
         <v>6</v>
       </c>
       <c r="J48" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="K48" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="M48" t="s">
         <v>105</v>
@@ -3527,7 +3524,7 @@
         <v>187</v>
       </c>
       <c r="O48" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="49" spans="1:16">
@@ -3553,16 +3550,16 @@
         <v>70</v>
       </c>
       <c r="H49" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I49" t="s">
         <v>6</v>
       </c>
       <c r="J49" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="K49" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="M49" t="s">
         <v>105</v>
@@ -3571,7 +3568,7 @@
         <v>187</v>
       </c>
       <c r="O49" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="50" spans="1:16">
@@ -3597,17 +3594,17 @@
         <v>70</v>
       </c>
       <c r="H50" t="s">
+        <v>201</v>
+      </c>
+      <c r="I50" t="s">
+        <v>6</v>
+      </c>
+      <c r="J50" t="s">
+        <v>255</v>
+      </c>
+      <c r="K50" t="s">
         <v>202</v>
       </c>
-      <c r="I50" t="s">
-        <v>6</v>
-      </c>
-      <c r="J50" t="s">
-        <v>256</v>
-      </c>
-      <c r="K50" t="s">
-        <v>203</v>
-      </c>
       <c r="M50" t="s">
         <v>105</v>
       </c>
@@ -3615,7 +3612,7 @@
         <v>187</v>
       </c>
       <c r="O50" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="51" spans="1:16">
@@ -3641,17 +3638,17 @@
         <v>70</v>
       </c>
       <c r="H51" t="s">
+        <v>201</v>
+      </c>
+      <c r="I51" t="s">
+        <v>6</v>
+      </c>
+      <c r="J51" t="s">
+        <v>255</v>
+      </c>
+      <c r="K51" t="s">
         <v>202</v>
       </c>
-      <c r="I51" t="s">
-        <v>6</v>
-      </c>
-      <c r="J51" t="s">
-        <v>256</v>
-      </c>
-      <c r="K51" t="s">
-        <v>203</v>
-      </c>
       <c r="M51" t="s">
         <v>105</v>
       </c>
@@ -3659,7 +3656,7 @@
         <v>187</v>
       </c>
       <c r="O51" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="52" spans="1:16">
@@ -3685,17 +3682,17 @@
         <v>70</v>
       </c>
       <c r="H52" t="s">
+        <v>201</v>
+      </c>
+      <c r="I52" t="s">
+        <v>6</v>
+      </c>
+      <c r="J52" t="s">
+        <v>255</v>
+      </c>
+      <c r="K52" t="s">
         <v>202</v>
       </c>
-      <c r="I52" t="s">
-        <v>6</v>
-      </c>
-      <c r="J52" t="s">
-        <v>256</v>
-      </c>
-      <c r="K52" t="s">
-        <v>203</v>
-      </c>
       <c r="M52" t="s">
         <v>105</v>
       </c>
@@ -3703,7 +3700,7 @@
         <v>187</v>
       </c>
       <c r="O52" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="53" spans="1:16">
@@ -3729,17 +3726,17 @@
         <v>70</v>
       </c>
       <c r="H53" t="s">
+        <v>201</v>
+      </c>
+      <c r="I53" t="s">
+        <v>6</v>
+      </c>
+      <c r="J53" t="s">
+        <v>255</v>
+      </c>
+      <c r="K53" t="s">
         <v>202</v>
       </c>
-      <c r="I53" t="s">
-        <v>6</v>
-      </c>
-      <c r="J53" t="s">
-        <v>256</v>
-      </c>
-      <c r="K53" t="s">
-        <v>203</v>
-      </c>
       <c r="M53" t="s">
         <v>105</v>
       </c>
@@ -3747,7 +3744,7 @@
         <v>187</v>
       </c>
       <c r="O53" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="54" spans="1:16">
@@ -3780,10 +3777,10 @@
         <v>6</v>
       </c>
       <c r="J54" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="K54" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="55" spans="1:16">
@@ -3809,17 +3806,17 @@
         <v>70</v>
       </c>
       <c r="H55" t="s">
+        <v>201</v>
+      </c>
+      <c r="I55" t="s">
+        <v>6</v>
+      </c>
+      <c r="J55" t="s">
+        <v>255</v>
+      </c>
+      <c r="K55" t="s">
         <v>202</v>
       </c>
-      <c r="I55" t="s">
-        <v>6</v>
-      </c>
-      <c r="J55" t="s">
-        <v>256</v>
-      </c>
-      <c r="K55" t="s">
-        <v>203</v>
-      </c>
       <c r="M55" t="s">
         <v>105</v>
       </c>
@@ -3827,7 +3824,7 @@
         <v>187</v>
       </c>
       <c r="O55" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="56" spans="1:16">
@@ -3853,17 +3850,17 @@
         <v>70</v>
       </c>
       <c r="H56" t="s">
+        <v>201</v>
+      </c>
+      <c r="I56" t="s">
+        <v>6</v>
+      </c>
+      <c r="J56" t="s">
+        <v>255</v>
+      </c>
+      <c r="K56" t="s">
         <v>202</v>
       </c>
-      <c r="I56" t="s">
-        <v>6</v>
-      </c>
-      <c r="J56" t="s">
-        <v>256</v>
-      </c>
-      <c r="K56" t="s">
-        <v>203</v>
-      </c>
       <c r="M56" t="s">
         <v>105</v>
       </c>
@@ -3871,7 +3868,7 @@
         <v>187</v>
       </c>
       <c r="O56" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="57" spans="1:16">
@@ -3904,7 +3901,7 @@
         <v>6</v>
       </c>
       <c r="J57" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="58" spans="1:16">
@@ -3930,17 +3927,17 @@
         <v>70</v>
       </c>
       <c r="H58" t="s">
+        <v>201</v>
+      </c>
+      <c r="I58" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="J58" t="s">
+        <v>255</v>
+      </c>
+      <c r="K58" t="s">
         <v>202</v>
       </c>
-      <c r="I58" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="J58" t="s">
-        <v>256</v>
-      </c>
-      <c r="K58" t="s">
-        <v>203</v>
-      </c>
       <c r="M58" t="s">
         <v>105</v>
       </c>
@@ -3948,7 +3945,7 @@
         <v>187</v>
       </c>
       <c r="O58" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="59" spans="1:16">
@@ -3974,19 +3971,19 @@
         <v>70</v>
       </c>
       <c r="H59" t="s">
+        <v>201</v>
+      </c>
+      <c r="I59" t="s">
+        <v>6</v>
+      </c>
+      <c r="J59" t="s">
+        <v>255</v>
+      </c>
+      <c r="K59" t="s">
         <v>202</v>
       </c>
-      <c r="I59" t="s">
-        <v>6</v>
-      </c>
-      <c r="J59" t="s">
-        <v>256</v>
-      </c>
-      <c r="K59" t="s">
-        <v>203</v>
-      </c>
       <c r="L59" s="7" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="M59" t="s">
         <v>105</v>
@@ -3995,7 +3992,7 @@
         <v>187</v>
       </c>
       <c r="O59" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="60" spans="1:16">
@@ -4021,17 +4018,17 @@
         <v>70</v>
       </c>
       <c r="H60" t="s">
+        <v>201</v>
+      </c>
+      <c r="I60" t="s">
+        <v>6</v>
+      </c>
+      <c r="J60" t="s">
+        <v>255</v>
+      </c>
+      <c r="K60" t="s">
         <v>202</v>
       </c>
-      <c r="I60" t="s">
-        <v>6</v>
-      </c>
-      <c r="J60" t="s">
-        <v>256</v>
-      </c>
-      <c r="K60" t="s">
-        <v>203</v>
-      </c>
       <c r="M60" t="s">
         <v>105</v>
       </c>
@@ -4039,7 +4036,7 @@
         <v>187</v>
       </c>
       <c r="O60" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="61" spans="1:16" ht="30">
@@ -4066,19 +4063,19 @@
         <v>70</v>
       </c>
       <c r="H61" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="I61" t="s">
         <v>6</v>
       </c>
       <c r="J61" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="K61" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="L61" s="7" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="M61" t="s">
         <v>105</v>
@@ -4113,17 +4110,17 @@
         <v>70</v>
       </c>
       <c r="H62" t="s">
+        <v>201</v>
+      </c>
+      <c r="I62" t="s">
+        <v>6</v>
+      </c>
+      <c r="J62" t="s">
+        <v>255</v>
+      </c>
+      <c r="K62" t="s">
         <v>202</v>
       </c>
-      <c r="I62" t="s">
-        <v>6</v>
-      </c>
-      <c r="J62" t="s">
-        <v>256</v>
-      </c>
-      <c r="K62" t="s">
-        <v>203</v>
-      </c>
       <c r="M62" t="s">
         <v>105</v>
       </c>
@@ -4131,7 +4128,7 @@
         <v>187</v>
       </c>
       <c r="O62" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="63" spans="1:16">
@@ -4157,17 +4154,17 @@
         <v>70</v>
       </c>
       <c r="H63" t="s">
+        <v>201</v>
+      </c>
+      <c r="I63" t="s">
+        <v>6</v>
+      </c>
+      <c r="J63" t="s">
+        <v>255</v>
+      </c>
+      <c r="K63" t="s">
         <v>202</v>
       </c>
-      <c r="I63" t="s">
-        <v>6</v>
-      </c>
-      <c r="J63" t="s">
-        <v>256</v>
-      </c>
-      <c r="K63" t="s">
-        <v>203</v>
-      </c>
       <c r="M63" t="s">
         <v>105</v>
       </c>
@@ -4175,7 +4172,7 @@
         <v>187</v>
       </c>
       <c r="O63" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="64" spans="1:16">
@@ -4201,19 +4198,19 @@
         <v>70</v>
       </c>
       <c r="H64" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="I64" t="s">
         <v>6</v>
       </c>
       <c r="J64" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="K64" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="L64" s="7" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="M64" t="s">
         <v>105</v>
@@ -4222,7 +4219,7 @@
         <v>187</v>
       </c>
       <c r="O64" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="65" spans="1:16">
@@ -4248,19 +4245,19 @@
         <v>70</v>
       </c>
       <c r="H65" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="I65" t="s">
         <v>6</v>
       </c>
       <c r="J65" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="K65" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="L65" s="7" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="M65" t="s">
         <v>105</v>
@@ -4269,7 +4266,7 @@
         <v>187</v>
       </c>
       <c r="O65" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="66" spans="1:16" ht="30">
@@ -4296,19 +4293,19 @@
         <v>70</v>
       </c>
       <c r="H66" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="I66" t="s">
         <v>6</v>
       </c>
       <c r="J66" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="K66" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="L66" s="7" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="M66" t="s">
         <v>105</v>
@@ -4341,16 +4338,16 @@
         <v>70</v>
       </c>
       <c r="H67" s="16" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="I67" s="16" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="J67" s="16" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="K67" s="16" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="L67" s="17"/>
       <c r="M67" s="16" t="s">
@@ -4384,19 +4381,19 @@
         <v>70</v>
       </c>
       <c r="H68" s="16" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="I68" s="16" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="J68" s="16" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="K68" s="16" t="s">
+        <v>212</v>
+      </c>
+      <c r="L68" s="17" t="s">
         <v>213</v>
-      </c>
-      <c r="L68" s="17" t="s">
-        <v>214</v>
       </c>
       <c r="M68" s="16" t="s">
         <v>105</v>
@@ -4429,19 +4426,19 @@
         <v>70</v>
       </c>
       <c r="H69" s="16" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="I69" s="16" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="J69" s="16" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="K69" s="16" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="L69" s="17" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="M69" s="16" t="s">
         <v>105</v>
@@ -4474,19 +4471,19 @@
         <v>70</v>
       </c>
       <c r="H70" s="16" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="I70" s="16" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="J70" s="16" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="K70" s="16" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="L70" s="17" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="M70" s="16" t="s">
         <v>105</v>
@@ -4519,19 +4516,19 @@
         <v>70</v>
       </c>
       <c r="H71" s="16" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="I71" s="16" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="J71" s="16" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="K71" s="16" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="L71" s="17" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="M71" s="16" t="s">
         <v>105</v>
@@ -4564,19 +4561,19 @@
         <v>70</v>
       </c>
       <c r="H72" s="16" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="I72" s="16" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="J72" s="16" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="K72" s="16" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="L72" s="17" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="M72" s="16" t="s">
         <v>105</v>
@@ -4609,19 +4606,19 @@
         <v>70</v>
       </c>
       <c r="H73" s="16" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="I73" s="16" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="J73" s="16" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="K73" s="16" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="L73" s="17" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="M73" s="16" t="s">
         <v>105</v>
@@ -4653,19 +4650,19 @@
         <v>70</v>
       </c>
       <c r="H74" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="I74" t="s">
         <v>6</v>
       </c>
       <c r="J74" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="K74" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="L74" s="8" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="M74" t="s">
         <v>105</v>
@@ -4674,7 +4671,7 @@
         <v>187</v>
       </c>
       <c r="O74" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="75" spans="1:16">
@@ -4700,19 +4697,19 @@
         <v>70</v>
       </c>
       <c r="H75" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="I75" t="s">
         <v>6</v>
       </c>
       <c r="J75" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="K75" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="L75" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="M75" t="s">
         <v>105</v>
@@ -4721,7 +4718,7 @@
         <v>187</v>
       </c>
       <c r="O75" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="76" spans="1:16" s="9" customFormat="1" ht="30">
@@ -4747,19 +4744,19 @@
         <v>70</v>
       </c>
       <c r="H76" s="9" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="I76" s="9" t="s">
         <v>6</v>
       </c>
       <c r="J76" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="K76" s="9" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="L76" s="8" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="M76" s="9" t="s">
         <v>105</v>
@@ -4768,7 +4765,7 @@
         <v>187</v>
       </c>
       <c r="O76" s="9" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="77" spans="1:16" s="9" customFormat="1">
@@ -4801,10 +4798,10 @@
         <v>6</v>
       </c>
       <c r="J77" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="K77" s="9" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="L77" s="8"/>
       <c r="P77" s="9" t="s">
@@ -4834,19 +4831,19 @@
         <v>70</v>
       </c>
       <c r="H78" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="I78" t="s">
         <v>6</v>
       </c>
       <c r="J78" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="K78" s="9" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="L78" s="7" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="M78" t="s">
         <v>105</v>
@@ -4855,7 +4852,7 @@
         <v>187</v>
       </c>
       <c r="O78" s="9" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="79" spans="1:16">
@@ -4881,19 +4878,19 @@
         <v>70</v>
       </c>
       <c r="H79" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="I79" s="9" t="s">
         <v>6</v>
       </c>
       <c r="J79" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="K79" s="9" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="L79" s="7" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="M79" t="s">
         <v>105</v>
@@ -4902,7 +4899,7 @@
         <v>187</v>
       </c>
       <c r="O79" s="9" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="80" spans="1:16">
@@ -4928,19 +4925,19 @@
         <v>70</v>
       </c>
       <c r="H80" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="I80" s="9" t="s">
         <v>6</v>
       </c>
       <c r="J80" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="K80" s="9" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="L80" s="7" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="M80" t="s">
         <v>105</v>
@@ -4949,7 +4946,7 @@
         <v>187</v>
       </c>
       <c r="O80" s="9" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="81" spans="1:16" s="16" customFormat="1">
@@ -4975,19 +4972,19 @@
         <v>70</v>
       </c>
       <c r="H81" s="16" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="I81" s="16" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="J81" s="16" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="K81" s="16" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="L81" s="17" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="M81" s="16" t="s">
         <v>105</v>
@@ -4996,7 +4993,7 @@
         <v>187</v>
       </c>
       <c r="O81" s="16" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="82" spans="1:16" s="9" customFormat="1">
@@ -5022,16 +5019,16 @@
         <v>70</v>
       </c>
       <c r="H82" s="9" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="I82" s="9" t="s">
         <v>6</v>
       </c>
       <c r="J82" s="9" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="K82" s="9" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="L82" s="8"/>
       <c r="M82" s="9" t="s">
@@ -5041,7 +5038,7 @@
         <v>187</v>
       </c>
       <c r="P82" s="9" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="83" spans="1:16">
@@ -5074,13 +5071,13 @@
         <v>6</v>
       </c>
       <c r="J83" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="K83" s="9" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="L83" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="84" spans="1:16">
@@ -5106,19 +5103,19 @@
         <v>70</v>
       </c>
       <c r="H84" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="I84" s="9" t="s">
         <v>6</v>
       </c>
       <c r="J84" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="K84" s="9" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="L84" s="8" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="M84" t="s">
         <v>105</v>
@@ -5127,7 +5124,7 @@
         <v>187</v>
       </c>
       <c r="O84" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="85" spans="1:16">
@@ -5160,10 +5157,10 @@
         <v>6</v>
       </c>
       <c r="J85" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="K85" s="9" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="86" spans="1:16">
@@ -5189,19 +5186,19 @@
         <v>70</v>
       </c>
       <c r="H86" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="I86" s="9" t="s">
         <v>6</v>
       </c>
       <c r="J86" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="K86" s="9" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="L86" s="7" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="M86" t="s">
         <v>105</v>
@@ -5210,7 +5207,7 @@
         <v>187</v>
       </c>
       <c r="P86" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="87" spans="1:16">
@@ -5243,13 +5240,13 @@
         <v>6</v>
       </c>
       <c r="J87" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="K87" s="9" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="L87" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="88" spans="1:16" ht="30">
@@ -5275,28 +5272,28 @@
         <v>70</v>
       </c>
       <c r="H88" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="I88" s="9" t="s">
         <v>6</v>
       </c>
       <c r="J88" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="K88" s="9" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="L88" s="8" t="s">
+        <v>274</v>
+      </c>
+      <c r="M88" t="s">
+        <v>105</v>
+      </c>
+      <c r="N88" t="s">
+        <v>187</v>
+      </c>
+      <c r="O88" t="s">
         <v>275</v>
-      </c>
-      <c r="M88" t="s">
-        <v>105</v>
-      </c>
-      <c r="N88" t="s">
-        <v>187</v>
-      </c>
-      <c r="O88" t="s">
-        <v>276</v>
       </c>
     </row>
     <row r="89" spans="1:16">
@@ -5329,13 +5326,13 @@
         <v>6</v>
       </c>
       <c r="J89" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="K89" s="9" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="L89" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="90" spans="1:16">
@@ -5362,19 +5359,19 @@
         <v>70</v>
       </c>
       <c r="H90" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="I90" s="9" t="s">
         <v>6</v>
       </c>
       <c r="J90" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="K90" s="12" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="L90" s="8" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="M90" t="s">
         <v>105</v>
@@ -5410,16 +5407,16 @@
         <v>70</v>
       </c>
       <c r="H91" t="s">
+        <v>211</v>
+      </c>
+      <c r="I91" t="s">
+        <v>6</v>
+      </c>
+      <c r="J91" t="s">
+        <v>255</v>
+      </c>
+      <c r="K91" t="s">
         <v>212</v>
-      </c>
-      <c r="I91" t="s">
-        <v>6</v>
-      </c>
-      <c r="J91" t="s">
-        <v>256</v>
-      </c>
-      <c r="K91" t="s">
-        <v>213</v>
       </c>
       <c r="L91" s="8"/>
       <c r="M91" t="s">
@@ -5462,7 +5459,7 @@
         <v>73</v>
       </c>
       <c r="K92" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="93" spans="1:16">
@@ -5489,19 +5486,19 @@
         <v>70</v>
       </c>
       <c r="H93" t="s">
+        <v>211</v>
+      </c>
+      <c r="I93" t="s">
+        <v>6</v>
+      </c>
+      <c r="J93" t="s">
+        <v>255</v>
+      </c>
+      <c r="K93" t="s">
         <v>212</v>
       </c>
-      <c r="I93" t="s">
-        <v>6</v>
-      </c>
-      <c r="J93" t="s">
-        <v>256</v>
-      </c>
-      <c r="K93" t="s">
-        <v>213</v>
-      </c>
       <c r="L93" s="8" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="M93" t="s">
         <v>105</v>
@@ -5515,7 +5512,7 @@
     </row>
     <row r="94" spans="1:16">
       <c r="A94" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B94" t="s">
         <v>11</v>
@@ -5546,7 +5543,7 @@
         <v>73</v>
       </c>
       <c r="K94" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="95" spans="1:16">
@@ -5582,7 +5579,7 @@
         <v>73</v>
       </c>
       <c r="K95" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="96" spans="1:16" ht="30">
@@ -5609,7 +5606,7 @@
         <v>70</v>
       </c>
       <c r="H96" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I96" t="s">
         <v>6</v>
@@ -5618,10 +5615,10 @@
         <v>73</v>
       </c>
       <c r="K96" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="L96" s="7" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="M96" t="s">
         <v>105</v>
@@ -5654,7 +5651,7 @@
         <v>70</v>
       </c>
       <c r="H97" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I97" t="s">
         <v>6</v>
@@ -5663,7 +5660,7 @@
         <v>73</v>
       </c>
       <c r="K97" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="M97" t="s">
         <v>105</v>
@@ -5699,7 +5696,7 @@
         <v>70</v>
       </c>
       <c r="H98" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I98" t="s">
         <v>6</v>
@@ -5708,7 +5705,7 @@
         <v>73</v>
       </c>
       <c r="K98" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="M98" t="s">
         <v>105</v>
@@ -5750,7 +5747,7 @@
         <v>73</v>
       </c>
       <c r="K99" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="M99" t="s">
         <v>105</v>
@@ -5795,10 +5792,10 @@
         <v>73</v>
       </c>
       <c r="K100" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="L100" s="7" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="M100" t="s">
         <v>105</v>
@@ -5840,7 +5837,7 @@
         <v>73</v>
       </c>
       <c r="K101" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="102" spans="1:16">
@@ -5876,10 +5873,10 @@
         <v>73</v>
       </c>
       <c r="K102" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="L102" s="7" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="M102" t="s">
         <v>105</v>
@@ -5921,10 +5918,10 @@
         <v>73</v>
       </c>
       <c r="K103" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="L103" s="7" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="104" spans="1:16">
@@ -5960,7 +5957,7 @@
         <v>73</v>
       </c>
       <c r="K104" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="M104" t="s">
         <v>105</v>
@@ -6002,7 +5999,7 @@
         <v>73</v>
       </c>
       <c r="K105" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="M105" t="s">
         <v>105</v>
@@ -6038,16 +6035,16 @@
         <v>73</v>
       </c>
       <c r="I106" s="16" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="J106" t="s">
         <v>73</v>
       </c>
       <c r="K106" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="L106" s="7" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="M106" t="s">
         <v>105</v>
@@ -6089,7 +6086,7 @@
         <v>73</v>
       </c>
       <c r="K107" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="108" spans="1:16">
@@ -6150,13 +6147,13 @@
         <v>73</v>
       </c>
       <c r="I109" s="16" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="J109" t="s">
         <v>73</v>
       </c>
       <c r="L109" s="7" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="110" spans="1:16">
@@ -6294,7 +6291,7 @@
         <v>73</v>
       </c>
       <c r="L113" s="7" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="114" spans="1:16">
@@ -6330,7 +6327,7 @@
         <v>73</v>
       </c>
       <c r="L114" s="7" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="P114" t="s">
         <v>6</v>
@@ -6402,7 +6399,7 @@
         <v>73</v>
       </c>
       <c r="L116" s="7" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="117" spans="1:16" ht="30">
@@ -6429,16 +6426,16 @@
         <v>70</v>
       </c>
       <c r="H117" t="s">
+        <v>194</v>
+      </c>
+      <c r="I117" s="16" t="s">
+        <v>257</v>
+      </c>
+      <c r="J117" t="s">
         <v>195</v>
       </c>
-      <c r="I117" s="16" t="s">
-        <v>258</v>
-      </c>
-      <c r="J117" t="s">
-        <v>196</v>
-      </c>
       <c r="L117" s="7" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="118" spans="1:16">
@@ -6465,13 +6462,13 @@
         <v>70</v>
       </c>
       <c r="H118" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="I118" s="9" t="s">
         <v>6</v>
       </c>
       <c r="J118" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="119" spans="1:16">
@@ -6498,13 +6495,13 @@
         <v>70</v>
       </c>
       <c r="H119" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="I119" s="9" t="s">
         <v>6</v>
       </c>
       <c r="J119" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="120" spans="1:16">
@@ -6531,13 +6528,13 @@
         <v>70</v>
       </c>
       <c r="H120" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="I120" s="9" t="s">
         <v>6</v>
       </c>
       <c r="L120" s="7" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="121" spans="1:16">
@@ -6564,7 +6561,7 @@
         <v>70</v>
       </c>
       <c r="H121" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="I121" s="9" t="s">
         <v>6</v>
@@ -6597,7 +6594,7 @@
         <v>70</v>
       </c>
       <c r="H122" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="I122" s="9" t="s">
         <v>6</v>
@@ -6627,7 +6624,7 @@
         <v>70</v>
       </c>
       <c r="H123" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="I123" s="9" t="s">
         <v>6</v>
@@ -6657,7 +6654,7 @@
         <v>70</v>
       </c>
       <c r="H124" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="I124" s="9" t="s">
         <v>6</v>
@@ -6685,10 +6682,10 @@
         <v>70</v>
       </c>
       <c r="H125" s="16" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="I125" s="16" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="L125" s="17"/>
       <c r="M125" s="16" t="s">
@@ -6722,7 +6719,7 @@
         <v>70</v>
       </c>
       <c r="H126" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="I126" s="9" t="s">
         <v>6</v>
@@ -6752,7 +6749,7 @@
         <v>70</v>
       </c>
       <c r="H127" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="I127" s="9" t="s">
         <v>6</v>
@@ -6782,7 +6779,7 @@
         <v>70</v>
       </c>
       <c r="H128" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="I128" s="9" t="s">
         <v>6</v>
@@ -6815,7 +6812,7 @@
         <v>70</v>
       </c>
       <c r="H129" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="I129" s="9" t="s">
         <v>6</v>
@@ -6849,7 +6846,7 @@
         <v>189</v>
       </c>
       <c r="I130" s="16" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="J130" s="16" t="s">
         <v>73</v>
@@ -6922,7 +6919,7 @@
         <v>70</v>
       </c>
       <c r="H132" s="9" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="I132" t="s">
         <v>6</v>
@@ -6952,7 +6949,7 @@
         <v>70</v>
       </c>
       <c r="H133" s="9" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="I133" t="s">
         <v>6</v>
@@ -6982,7 +6979,7 @@
         <v>70</v>
       </c>
       <c r="H134" s="9" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="I134" t="s">
         <v>6</v>
@@ -7012,7 +7009,7 @@
         <v>70</v>
       </c>
       <c r="H135" s="9" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="I135" t="s">
         <v>6</v>
@@ -7040,10 +7037,10 @@
         <v>70</v>
       </c>
       <c r="H136" s="16" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="I136" s="16" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="L136" s="17"/>
       <c r="M136" s="16" t="s">
@@ -7077,7 +7074,7 @@
         <v>70</v>
       </c>
       <c r="H137" s="9" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="I137" t="s">
         <v>6</v>
@@ -7104,13 +7101,13 @@
         <v>70</v>
       </c>
       <c r="H138" s="16" t="s">
+        <v>280</v>
+      </c>
+      <c r="I138" s="16" t="s">
+        <v>257</v>
+      </c>
+      <c r="L138" s="17" t="s">
         <v>281</v>
-      </c>
-      <c r="I138" s="16" t="s">
-        <v>258</v>
-      </c>
-      <c r="L138" s="17" t="s">
-        <v>282</v>
       </c>
       <c r="P138" s="16" t="s">
         <v>6</v>
@@ -7140,7 +7137,7 @@
         <v>70</v>
       </c>
       <c r="H139" s="9" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="I139" t="s">
         <v>6</v>
@@ -7173,7 +7170,7 @@
         <v>70</v>
       </c>
       <c r="H140" s="9" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="I140" s="9" t="s">
         <v>6</v>
@@ -7203,7 +7200,7 @@
         <v>70</v>
       </c>
       <c r="H141" s="9" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="I141" s="9" t="s">
         <v>6</v>
@@ -7236,7 +7233,7 @@
         <v>70</v>
       </c>
       <c r="H142" s="9" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="I142" s="9" t="s">
         <v>6</v>
@@ -7266,7 +7263,7 @@
         <v>70</v>
       </c>
       <c r="H143" s="9" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="I143" s="9" t="s">
         <v>6</v>
@@ -7302,7 +7299,7 @@
         <v>70</v>
       </c>
       <c r="H144" s="9" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="I144" s="9" t="s">
         <v>6</v>
@@ -7338,7 +7335,7 @@
         <v>70</v>
       </c>
       <c r="H145" s="9" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="I145" s="9" t="s">
         <v>6</v>
@@ -7368,7 +7365,7 @@
         <v>70</v>
       </c>
       <c r="H146" s="9" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="I146" s="9" t="s">
         <v>6</v>
@@ -7401,7 +7398,7 @@
         <v>70</v>
       </c>
       <c r="H147" s="9" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="I147" s="9" t="s">
         <v>6</v>
@@ -7443,7 +7440,7 @@
         <v>73</v>
       </c>
       <c r="L148" s="7" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="P148" t="s">
         <v>6</v>
@@ -7473,7 +7470,7 @@
         <v>70</v>
       </c>
       <c r="H149" s="9" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="I149" t="s">
         <v>6</v>
@@ -7542,7 +7539,7 @@
         <v>70</v>
       </c>
       <c r="H151" s="9" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="I151" t="s">
         <v>6</v>
@@ -7575,7 +7572,7 @@
         <v>70</v>
       </c>
       <c r="H152" s="9" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="I152" t="s">
         <v>6</v>
@@ -7608,7 +7605,7 @@
         <v>70</v>
       </c>
       <c r="H153" s="9" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="I153" t="s">
         <v>6</v>
@@ -7641,7 +7638,7 @@
         <v>70</v>
       </c>
       <c r="H154" s="9" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="I154" t="s">
         <v>6</v>
@@ -7671,13 +7668,13 @@
         <v>70</v>
       </c>
       <c r="H155" s="9" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="I155" t="s">
         <v>6</v>
       </c>
       <c r="L155" s="7" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="P155" t="s">
         <v>6</v>
@@ -7707,7 +7704,7 @@
         <v>70</v>
       </c>
       <c r="H156" s="9" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="I156" t="s">
         <v>6</v>
@@ -7740,7 +7737,7 @@
         <v>190</v>
       </c>
       <c r="L157" s="23" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="M157" s="20" t="s">
         <v>105</v>
@@ -7773,7 +7770,7 @@
         <v>70</v>
       </c>
       <c r="H158" s="9" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="I158" t="s">
         <v>6</v>
@@ -7803,7 +7800,7 @@
         <v>70</v>
       </c>
       <c r="H159" s="9" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="I159" t="s">
         <v>6</v>
@@ -7836,10 +7833,10 @@
         <v>70</v>
       </c>
       <c r="H160" s="16" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="I160" s="16" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="L160" s="17"/>
       <c r="M160" s="16" t="s">
@@ -7873,10 +7870,10 @@
         <v>70</v>
       </c>
       <c r="H161" s="16" t="s">
-        <v>191</v>
+        <v>280</v>
       </c>
       <c r="I161" s="16" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="L161" s="17"/>
       <c r="M161" s="16" t="s">
@@ -8051,7 +8048,7 @@
         <v>73</v>
       </c>
       <c r="L166" s="7" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="M166" t="s">
         <v>105</v>

</xml_diff>

<commit_message>
Finished ew.issue.19180413 on 5/4/2017, moved to tei_final; updated spreadsheet
</commit_message>
<xml_diff>
--- a/spreadsheet/EW.xlsx
+++ b/spreadsheet/EW.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1435" uniqueCount="284">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1435" uniqueCount="282">
   <si>
     <t>File Name</t>
   </si>
@@ -601,9 +601,6 @@
     <t>KH/LW</t>
   </si>
   <si>
-    <t>KH/</t>
-  </si>
-  <si>
     <t>CHO/LW</t>
   </si>
   <si>
@@ -878,9 +875,6 @@
   </si>
   <si>
     <t>4 extra pages</t>
-  </si>
-  <si>
-    <t>cannot find this file</t>
   </si>
 </sst>
 </file>
@@ -1024,15 +1018,15 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="16" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="16" fontId="5" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="16" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1348,8 +1342,8 @@
   </sheetPr>
   <dimension ref="A1:Q168"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A136" zoomScaleNormal="100" zoomScalePageLayoutView="159" workbookViewId="0">
-      <selection activeCell="J165" sqref="J165"/>
+    <sheetView tabSelected="1" topLeftCell="A121" zoomScaleNormal="100" zoomScalePageLayoutView="159" workbookViewId="0">
+      <selection activeCell="H144" sqref="H144"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -1376,19 +1370,19 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>258</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="D1" s="5" t="s">
         <v>259</v>
       </c>
-      <c r="D1" s="5" t="s">
-        <v>260</v>
-      </c>
       <c r="E1" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>1</v>
@@ -1397,13 +1391,13 @@
         <v>2</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="J1" s="2" t="s">
         <v>3</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="L1" s="5" t="s">
         <v>58</v>
@@ -1415,13 +1409,13 @@
         <v>183</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="P1" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="Q1" s="1" t="s">
         <v>277</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>278</v>
       </c>
     </row>
     <row r="2" spans="1:17" s="3" customFormat="1">
@@ -1481,19 +1475,19 @@
         <v>71</v>
       </c>
       <c r="H3" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="I3" s="11" t="s">
         <v>6</v>
       </c>
       <c r="J3" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="K3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="L3" s="7" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="M3" t="s">
         <v>105</v>
@@ -1502,7 +1496,7 @@
         <v>187</v>
       </c>
       <c r="O3" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="4" spans="1:17" ht="75">
@@ -1528,19 +1522,19 @@
         <v>71</v>
       </c>
       <c r="H4" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="I4" s="9" t="s">
         <v>6</v>
       </c>
       <c r="J4" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="K4" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="L4" s="7" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="M4" t="s">
         <v>105</v>
@@ -1549,7 +1543,7 @@
         <v>187</v>
       </c>
       <c r="O4" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="5" spans="1:17" ht="60">
@@ -1575,19 +1569,19 @@
         <v>71</v>
       </c>
       <c r="H5" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="I5" s="9" t="s">
         <v>6</v>
       </c>
       <c r="J5" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="K5" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="L5" s="7" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="M5" t="s">
         <v>105</v>
@@ -1596,7 +1590,7 @@
         <v>187</v>
       </c>
       <c r="O5" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="6" spans="1:17">
@@ -1622,16 +1616,16 @@
         <v>185</v>
       </c>
       <c r="H6" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="I6" t="s">
         <v>6</v>
       </c>
       <c r="J6" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="K6" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="M6" t="s">
         <v>105</v>
@@ -1640,7 +1634,7 @@
         <v>187</v>
       </c>
       <c r="O6" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="7" spans="1:17">
@@ -1666,16 +1660,16 @@
         <v>186</v>
       </c>
       <c r="H7" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="I7" t="s">
         <v>6</v>
       </c>
       <c r="J7" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="K7" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="M7" t="s">
         <v>105</v>
@@ -1684,7 +1678,7 @@
         <v>187</v>
       </c>
       <c r="O7" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="8" spans="1:17">
@@ -1710,16 +1704,16 @@
         <v>185</v>
       </c>
       <c r="H8" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="I8" t="s">
         <v>6</v>
       </c>
       <c r="J8" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="K8" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="M8" t="s">
         <v>105</v>
@@ -1728,7 +1722,7 @@
         <v>187</v>
       </c>
       <c r="O8" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="9" spans="1:17">
@@ -1754,16 +1748,16 @@
         <v>185</v>
       </c>
       <c r="H9" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="I9" t="s">
         <v>6</v>
       </c>
       <c r="J9" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="K9" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="M9" t="s">
         <v>105</v>
@@ -1772,7 +1766,7 @@
         <v>187</v>
       </c>
       <c r="O9" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="10" spans="1:17">
@@ -1798,19 +1792,19 @@
         <v>185</v>
       </c>
       <c r="H10" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="I10" t="s">
         <v>6</v>
       </c>
       <c r="J10" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="K10" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="L10" s="7" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="M10" t="s">
         <v>105</v>
@@ -1819,7 +1813,7 @@
         <v>187</v>
       </c>
       <c r="O10" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="11" spans="1:17">
@@ -1845,16 +1839,16 @@
         <v>185</v>
       </c>
       <c r="H11" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="I11" t="s">
         <v>6</v>
       </c>
       <c r="J11" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="K11" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="M11" t="s">
         <v>105</v>
@@ -1863,7 +1857,7 @@
         <v>187</v>
       </c>
       <c r="O11" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="12" spans="1:17" ht="30">
@@ -1889,19 +1883,19 @@
         <v>188</v>
       </c>
       <c r="H12" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="I12" t="s">
         <v>6</v>
       </c>
       <c r="J12" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="K12" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="L12" s="7" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="M12" t="s">
         <v>105</v>
@@ -1910,7 +1904,7 @@
         <v>187</v>
       </c>
       <c r="O12" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="13" spans="1:17" ht="45">
@@ -1936,19 +1930,19 @@
         <v>188</v>
       </c>
       <c r="H13" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="I13" s="9" t="s">
         <v>6</v>
       </c>
       <c r="J13" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="K13" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="L13" s="7" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="M13" t="s">
         <v>105</v>
@@ -1957,7 +1951,7 @@
         <v>187</v>
       </c>
       <c r="O13" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="14" spans="1:17">
@@ -1983,16 +1977,16 @@
         <v>188</v>
       </c>
       <c r="H14" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="I14" t="s">
         <v>6</v>
       </c>
       <c r="J14" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="K14" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="M14" t="s">
         <v>105</v>
@@ -2001,7 +1995,7 @@
         <v>187</v>
       </c>
       <c r="O14" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="15" spans="1:17">
@@ -2027,19 +2021,19 @@
         <v>188</v>
       </c>
       <c r="H15" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="I15" t="s">
         <v>6</v>
       </c>
       <c r="J15" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="K15" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="L15" s="7" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="M15" t="s">
         <v>105</v>
@@ -2048,7 +2042,7 @@
         <v>187</v>
       </c>
       <c r="O15" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="16" spans="1:17">
@@ -2074,19 +2068,19 @@
         <v>188</v>
       </c>
       <c r="H16" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="I16" t="s">
         <v>6</v>
       </c>
       <c r="J16" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="K16" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="L16" s="7" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="M16" t="s">
         <v>105</v>
@@ -2095,7 +2089,7 @@
         <v>187</v>
       </c>
       <c r="O16" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="17" spans="1:16">
@@ -2121,16 +2115,16 @@
         <v>188</v>
       </c>
       <c r="H17" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="I17" t="s">
         <v>6</v>
       </c>
       <c r="J17" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="K17" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="M17" t="s">
         <v>105</v>
@@ -2139,7 +2133,7 @@
         <v>187</v>
       </c>
       <c r="O17" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="18" spans="1:16">
@@ -2175,10 +2169,10 @@
         <v>73</v>
       </c>
       <c r="K18" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="L18" s="7" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="19" spans="1:16">
@@ -2204,16 +2198,16 @@
         <v>188</v>
       </c>
       <c r="H19" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="I19" t="s">
         <v>6</v>
       </c>
       <c r="J19" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="K19" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="M19" t="s">
         <v>105</v>
@@ -2222,7 +2216,7 @@
         <v>187</v>
       </c>
       <c r="O19" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="20" spans="1:16">
@@ -2248,19 +2242,19 @@
         <v>188</v>
       </c>
       <c r="H20" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="I20" t="s">
         <v>6</v>
       </c>
       <c r="J20" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="K20" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="L20" s="7" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="M20" t="s">
         <v>105</v>
@@ -2269,7 +2263,7 @@
         <v>187</v>
       </c>
       <c r="O20" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="21" spans="1:16">
@@ -2295,16 +2289,16 @@
         <v>188</v>
       </c>
       <c r="H21" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="I21" t="s">
         <v>6</v>
       </c>
       <c r="J21" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="K21" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="M21" t="s">
         <v>105</v>
@@ -2313,7 +2307,7 @@
         <v>187</v>
       </c>
       <c r="O21" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="22" spans="1:16">
@@ -2339,16 +2333,16 @@
         <v>188</v>
       </c>
       <c r="H22" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="I22" t="s">
         <v>6</v>
       </c>
       <c r="J22" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="K22" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="M22" t="s">
         <v>105</v>
@@ -2357,7 +2351,7 @@
         <v>187</v>
       </c>
       <c r="O22" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="23" spans="1:16">
@@ -2383,16 +2377,16 @@
         <v>188</v>
       </c>
       <c r="H23" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="I23" t="s">
         <v>6</v>
       </c>
       <c r="J23" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="K23" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="M23" t="s">
         <v>105</v>
@@ -2401,7 +2395,7 @@
         <v>187</v>
       </c>
       <c r="O23" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="24" spans="1:16">
@@ -2437,7 +2431,7 @@
         <v>73</v>
       </c>
       <c r="K24" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="25" spans="1:16">
@@ -2463,16 +2457,16 @@
         <v>188</v>
       </c>
       <c r="H25" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="I25" t="s">
         <v>6</v>
       </c>
       <c r="J25" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="K25" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="M25" t="s">
         <v>105</v>
@@ -2481,7 +2475,7 @@
         <v>187</v>
       </c>
       <c r="O25" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="26" spans="1:16">
@@ -2507,16 +2501,16 @@
         <v>188</v>
       </c>
       <c r="H26" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="I26" t="s">
         <v>6</v>
       </c>
       <c r="J26" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="K26" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="M26" t="s">
         <v>105</v>
@@ -2525,7 +2519,7 @@
         <v>187</v>
       </c>
       <c r="O26" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="27" spans="1:16">
@@ -2552,16 +2546,16 @@
         <v>188</v>
       </c>
       <c r="H27" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="I27" t="s">
         <v>6</v>
       </c>
       <c r="J27" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="K27" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="M27" t="s">
         <v>105</v>
@@ -2593,13 +2587,13 @@
         <v>188</v>
       </c>
       <c r="H28" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="I28" t="s">
         <v>6</v>
       </c>
       <c r="J28" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="M28" t="s">
         <v>105</v>
@@ -2608,7 +2602,7 @@
         <v>187</v>
       </c>
       <c r="O28" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="29" spans="1:16" ht="30">
@@ -2634,19 +2628,19 @@
         <v>188</v>
       </c>
       <c r="H29" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="I29" t="s">
         <v>6</v>
       </c>
       <c r="J29" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="K29" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="L29" s="7" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="M29" t="s">
         <v>105</v>
@@ -2655,7 +2649,7 @@
         <v>187</v>
       </c>
       <c r="O29" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="30" spans="1:16" ht="45">
@@ -2681,19 +2675,19 @@
         <v>188</v>
       </c>
       <c r="H30" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="I30" t="s">
         <v>6</v>
       </c>
       <c r="J30" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="K30" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="L30" s="7" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="M30" t="s">
         <v>105</v>
@@ -2702,7 +2696,7 @@
         <v>187</v>
       </c>
       <c r="P30" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="31" spans="1:16" ht="30">
@@ -2728,19 +2722,19 @@
         <v>188</v>
       </c>
       <c r="H31" s="16" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="I31" s="18" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="J31" s="16" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="K31" s="16" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="L31" s="17" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="M31" s="16" t="s">
         <v>105</v>
@@ -2749,7 +2743,7 @@
         <v>187</v>
       </c>
       <c r="O31" s="16" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="32" spans="1:16">
@@ -2775,19 +2769,19 @@
         <v>188</v>
       </c>
       <c r="H32" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="I32" t="s">
         <v>6</v>
       </c>
       <c r="J32" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="K32" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="L32" s="7" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="M32" t="s">
         <v>105</v>
@@ -2796,7 +2790,7 @@
         <v>187</v>
       </c>
       <c r="O32" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="33" spans="1:16">
@@ -2822,16 +2816,16 @@
         <v>188</v>
       </c>
       <c r="H33" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="I33" t="s">
         <v>6</v>
       </c>
       <c r="J33" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="K33" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="M33" t="s">
         <v>105</v>
@@ -2840,7 +2834,7 @@
         <v>187</v>
       </c>
       <c r="P33" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="34" spans="1:16">
@@ -2866,16 +2860,16 @@
         <v>188</v>
       </c>
       <c r="H34" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="I34" t="s">
         <v>6</v>
       </c>
       <c r="J34" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="K34" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="M34" t="s">
         <v>105</v>
@@ -2884,7 +2878,7 @@
         <v>187</v>
       </c>
       <c r="O34" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="35" spans="1:16">
@@ -2910,19 +2904,19 @@
         <v>188</v>
       </c>
       <c r="H35" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="I35" t="s">
         <v>6</v>
       </c>
       <c r="J35" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="K35" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="L35" s="7" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="M35" t="s">
         <v>105</v>
@@ -2931,7 +2925,7 @@
         <v>187</v>
       </c>
       <c r="O35" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="36" spans="1:16">
@@ -2957,16 +2951,16 @@
         <v>188</v>
       </c>
       <c r="H36" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="I36" t="s">
         <v>6</v>
       </c>
       <c r="J36" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="K36" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="M36" t="s">
         <v>105</v>
@@ -2975,7 +2969,7 @@
         <v>187</v>
       </c>
       <c r="O36" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="37" spans="1:16">
@@ -3001,20 +2995,20 @@
         <v>188</v>
       </c>
       <c r="H37" t="s">
+        <v>191</v>
+      </c>
+      <c r="I37" t="s">
+        <v>6</v>
+      </c>
+      <c r="J37" t="s">
+        <v>254</v>
+      </c>
+      <c r="K37" t="s">
+        <v>201</v>
+      </c>
+      <c r="L37" s="7" t="s">
         <v>192</v>
       </c>
-      <c r="I37" t="s">
-        <v>6</v>
-      </c>
-      <c r="J37" t="s">
-        <v>255</v>
-      </c>
-      <c r="K37" t="s">
-        <v>202</v>
-      </c>
-      <c r="L37" s="7" t="s">
-        <v>193</v>
-      </c>
       <c r="M37" t="s">
         <v>105</v>
       </c>
@@ -3022,7 +3016,7 @@
         <v>187</v>
       </c>
       <c r="O37" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="38" spans="1:16" s="16" customFormat="1" ht="30">
@@ -3048,19 +3042,19 @@
         <v>188</v>
       </c>
       <c r="H38" s="16" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="I38" s="16" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="J38" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="K38" s="16" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="L38" s="17" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="M38" s="16" t="s">
         <v>105</v>
@@ -3069,7 +3063,7 @@
         <v>187</v>
       </c>
       <c r="O38" s="16" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="39" spans="1:16">
@@ -3095,19 +3089,19 @@
         <v>188</v>
       </c>
       <c r="H39" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="I39" t="s">
         <v>6</v>
       </c>
       <c r="J39" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="K39" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="L39" s="7" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="M39" t="s">
         <v>105</v>
@@ -3116,7 +3110,7 @@
         <v>187</v>
       </c>
       <c r="O39" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="40" spans="1:16">
@@ -3142,19 +3136,19 @@
         <v>188</v>
       </c>
       <c r="H40" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="I40" t="s">
         <v>6</v>
       </c>
       <c r="J40" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="K40" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="L40" s="7" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="M40" t="s">
         <v>105</v>
@@ -3163,7 +3157,7 @@
         <v>187</v>
       </c>
       <c r="O40" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="41" spans="1:16">
@@ -3189,19 +3183,19 @@
         <v>188</v>
       </c>
       <c r="H41" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="I41" t="s">
         <v>6</v>
       </c>
       <c r="J41" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="K41" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="L41" s="7" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="M41" t="s">
         <v>105</v>
@@ -3210,7 +3204,7 @@
         <v>187</v>
       </c>
       <c r="O41" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="42" spans="1:16">
@@ -3236,19 +3230,19 @@
         <v>188</v>
       </c>
       <c r="H42" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="I42" t="s">
         <v>6</v>
       </c>
       <c r="J42" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="K42" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="L42" s="7" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="M42" t="s">
         <v>105</v>
@@ -3257,7 +3251,7 @@
         <v>187</v>
       </c>
       <c r="O42" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="43" spans="1:16">
@@ -3283,19 +3277,19 @@
         <v>188</v>
       </c>
       <c r="H43" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="I43" t="s">
         <v>6</v>
       </c>
       <c r="J43" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="K43" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="L43" s="15" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="M43" t="s">
         <v>105</v>
@@ -3304,7 +3298,7 @@
         <v>187</v>
       </c>
       <c r="O43" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="44" spans="1:16">
@@ -3330,16 +3324,16 @@
         <v>188</v>
       </c>
       <c r="H44" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="I44" t="s">
         <v>6</v>
       </c>
       <c r="J44" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="K44" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="M44" t="s">
         <v>105</v>
@@ -3348,7 +3342,7 @@
         <v>187</v>
       </c>
       <c r="O44" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="45" spans="1:16">
@@ -3374,16 +3368,16 @@
         <v>188</v>
       </c>
       <c r="H45" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="I45" t="s">
         <v>6</v>
       </c>
       <c r="J45" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="K45" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="M45" t="s">
         <v>105</v>
@@ -3392,7 +3386,7 @@
         <v>187</v>
       </c>
       <c r="O45" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="46" spans="1:16">
@@ -3418,16 +3412,16 @@
         <v>188</v>
       </c>
       <c r="H46" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="I46" t="s">
         <v>6</v>
       </c>
       <c r="J46" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="K46" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="M46" t="s">
         <v>105</v>
@@ -3436,7 +3430,7 @@
         <v>187</v>
       </c>
       <c r="O46" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="47" spans="1:16">
@@ -3462,16 +3456,16 @@
         <v>188</v>
       </c>
       <c r="H47" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="I47" t="s">
         <v>6</v>
       </c>
       <c r="J47" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="K47" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="M47" t="s">
         <v>105</v>
@@ -3480,7 +3474,7 @@
         <v>187</v>
       </c>
       <c r="O47" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="48" spans="1:16">
@@ -3506,16 +3500,16 @@
         <v>188</v>
       </c>
       <c r="H48" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="I48" t="s">
         <v>6</v>
       </c>
       <c r="J48" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="K48" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="M48" t="s">
         <v>105</v>
@@ -3524,7 +3518,7 @@
         <v>187</v>
       </c>
       <c r="O48" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="49" spans="1:16">
@@ -3550,16 +3544,16 @@
         <v>70</v>
       </c>
       <c r="H49" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="I49" t="s">
         <v>6</v>
       </c>
       <c r="J49" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="K49" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="M49" t="s">
         <v>105</v>
@@ -3568,7 +3562,7 @@
         <v>187</v>
       </c>
       <c r="O49" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="50" spans="1:16">
@@ -3594,17 +3588,17 @@
         <v>70</v>
       </c>
       <c r="H50" t="s">
+        <v>200</v>
+      </c>
+      <c r="I50" t="s">
+        <v>6</v>
+      </c>
+      <c r="J50" t="s">
+        <v>254</v>
+      </c>
+      <c r="K50" t="s">
         <v>201</v>
       </c>
-      <c r="I50" t="s">
-        <v>6</v>
-      </c>
-      <c r="J50" t="s">
-        <v>255</v>
-      </c>
-      <c r="K50" t="s">
-        <v>202</v>
-      </c>
       <c r="M50" t="s">
         <v>105</v>
       </c>
@@ -3612,7 +3606,7 @@
         <v>187</v>
       </c>
       <c r="O50" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="51" spans="1:16">
@@ -3638,17 +3632,17 @@
         <v>70</v>
       </c>
       <c r="H51" t="s">
+        <v>200</v>
+      </c>
+      <c r="I51" t="s">
+        <v>6</v>
+      </c>
+      <c r="J51" t="s">
+        <v>254</v>
+      </c>
+      <c r="K51" t="s">
         <v>201</v>
       </c>
-      <c r="I51" t="s">
-        <v>6</v>
-      </c>
-      <c r="J51" t="s">
-        <v>255</v>
-      </c>
-      <c r="K51" t="s">
-        <v>202</v>
-      </c>
       <c r="M51" t="s">
         <v>105</v>
       </c>
@@ -3656,7 +3650,7 @@
         <v>187</v>
       </c>
       <c r="O51" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="52" spans="1:16">
@@ -3682,17 +3676,17 @@
         <v>70</v>
       </c>
       <c r="H52" t="s">
+        <v>200</v>
+      </c>
+      <c r="I52" t="s">
+        <v>6</v>
+      </c>
+      <c r="J52" t="s">
+        <v>254</v>
+      </c>
+      <c r="K52" t="s">
         <v>201</v>
       </c>
-      <c r="I52" t="s">
-        <v>6</v>
-      </c>
-      <c r="J52" t="s">
-        <v>255</v>
-      </c>
-      <c r="K52" t="s">
-        <v>202</v>
-      </c>
       <c r="M52" t="s">
         <v>105</v>
       </c>
@@ -3700,7 +3694,7 @@
         <v>187</v>
       </c>
       <c r="O52" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="53" spans="1:16">
@@ -3726,17 +3720,17 @@
         <v>70</v>
       </c>
       <c r="H53" t="s">
+        <v>200</v>
+      </c>
+      <c r="I53" t="s">
+        <v>6</v>
+      </c>
+      <c r="J53" t="s">
+        <v>254</v>
+      </c>
+      <c r="K53" t="s">
         <v>201</v>
       </c>
-      <c r="I53" t="s">
-        <v>6</v>
-      </c>
-      <c r="J53" t="s">
-        <v>255</v>
-      </c>
-      <c r="K53" t="s">
-        <v>202</v>
-      </c>
       <c r="M53" t="s">
         <v>105</v>
       </c>
@@ -3744,7 +3738,7 @@
         <v>187</v>
       </c>
       <c r="O53" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="54" spans="1:16">
@@ -3777,10 +3771,10 @@
         <v>6</v>
       </c>
       <c r="J54" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="K54" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="55" spans="1:16">
@@ -3806,17 +3800,17 @@
         <v>70</v>
       </c>
       <c r="H55" t="s">
+        <v>200</v>
+      </c>
+      <c r="I55" t="s">
+        <v>6</v>
+      </c>
+      <c r="J55" t="s">
+        <v>254</v>
+      </c>
+      <c r="K55" t="s">
         <v>201</v>
       </c>
-      <c r="I55" t="s">
-        <v>6</v>
-      </c>
-      <c r="J55" t="s">
-        <v>255</v>
-      </c>
-      <c r="K55" t="s">
-        <v>202</v>
-      </c>
       <c r="M55" t="s">
         <v>105</v>
       </c>
@@ -3824,7 +3818,7 @@
         <v>187</v>
       </c>
       <c r="O55" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="56" spans="1:16">
@@ -3850,17 +3844,17 @@
         <v>70</v>
       </c>
       <c r="H56" t="s">
+        <v>200</v>
+      </c>
+      <c r="I56" t="s">
+        <v>6</v>
+      </c>
+      <c r="J56" t="s">
+        <v>254</v>
+      </c>
+      <c r="K56" t="s">
         <v>201</v>
       </c>
-      <c r="I56" t="s">
-        <v>6</v>
-      </c>
-      <c r="J56" t="s">
-        <v>255</v>
-      </c>
-      <c r="K56" t="s">
-        <v>202</v>
-      </c>
       <c r="M56" t="s">
         <v>105</v>
       </c>
@@ -3868,7 +3862,7 @@
         <v>187</v>
       </c>
       <c r="O56" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="57" spans="1:16">
@@ -3901,7 +3895,7 @@
         <v>6</v>
       </c>
       <c r="J57" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="58" spans="1:16">
@@ -3927,17 +3921,17 @@
         <v>70</v>
       </c>
       <c r="H58" t="s">
+        <v>200</v>
+      </c>
+      <c r="I58" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="J58" t="s">
+        <v>254</v>
+      </c>
+      <c r="K58" t="s">
         <v>201</v>
       </c>
-      <c r="I58" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="J58" t="s">
-        <v>255</v>
-      </c>
-      <c r="K58" t="s">
-        <v>202</v>
-      </c>
       <c r="M58" t="s">
         <v>105</v>
       </c>
@@ -3945,7 +3939,7 @@
         <v>187</v>
       </c>
       <c r="O58" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="59" spans="1:16">
@@ -3971,19 +3965,19 @@
         <v>70</v>
       </c>
       <c r="H59" t="s">
+        <v>200</v>
+      </c>
+      <c r="I59" t="s">
+        <v>6</v>
+      </c>
+      <c r="J59" t="s">
+        <v>254</v>
+      </c>
+      <c r="K59" t="s">
         <v>201</v>
       </c>
-      <c r="I59" t="s">
-        <v>6</v>
-      </c>
-      <c r="J59" t="s">
-        <v>255</v>
-      </c>
-      <c r="K59" t="s">
-        <v>202</v>
-      </c>
       <c r="L59" s="7" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="M59" t="s">
         <v>105</v>
@@ -3992,7 +3986,7 @@
         <v>187</v>
       </c>
       <c r="O59" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="60" spans="1:16">
@@ -4018,17 +4012,17 @@
         <v>70</v>
       </c>
       <c r="H60" t="s">
+        <v>200</v>
+      </c>
+      <c r="I60" t="s">
+        <v>6</v>
+      </c>
+      <c r="J60" t="s">
+        <v>254</v>
+      </c>
+      <c r="K60" t="s">
         <v>201</v>
       </c>
-      <c r="I60" t="s">
-        <v>6</v>
-      </c>
-      <c r="J60" t="s">
-        <v>255</v>
-      </c>
-      <c r="K60" t="s">
-        <v>202</v>
-      </c>
       <c r="M60" t="s">
         <v>105</v>
       </c>
@@ -4036,7 +4030,7 @@
         <v>187</v>
       </c>
       <c r="O60" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="61" spans="1:16" ht="30">
@@ -4063,19 +4057,19 @@
         <v>70</v>
       </c>
       <c r="H61" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="I61" t="s">
         <v>6</v>
       </c>
       <c r="J61" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="K61" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="L61" s="7" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="M61" t="s">
         <v>105</v>
@@ -4110,17 +4104,17 @@
         <v>70</v>
       </c>
       <c r="H62" t="s">
+        <v>200</v>
+      </c>
+      <c r="I62" t="s">
+        <v>6</v>
+      </c>
+      <c r="J62" t="s">
+        <v>254</v>
+      </c>
+      <c r="K62" t="s">
         <v>201</v>
       </c>
-      <c r="I62" t="s">
-        <v>6</v>
-      </c>
-      <c r="J62" t="s">
-        <v>255</v>
-      </c>
-      <c r="K62" t="s">
-        <v>202</v>
-      </c>
       <c r="M62" t="s">
         <v>105</v>
       </c>
@@ -4128,7 +4122,7 @@
         <v>187</v>
       </c>
       <c r="O62" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="63" spans="1:16">
@@ -4154,17 +4148,17 @@
         <v>70</v>
       </c>
       <c r="H63" t="s">
+        <v>200</v>
+      </c>
+      <c r="I63" t="s">
+        <v>6</v>
+      </c>
+      <c r="J63" t="s">
+        <v>254</v>
+      </c>
+      <c r="K63" t="s">
         <v>201</v>
       </c>
-      <c r="I63" t="s">
-        <v>6</v>
-      </c>
-      <c r="J63" t="s">
-        <v>255</v>
-      </c>
-      <c r="K63" t="s">
-        <v>202</v>
-      </c>
       <c r="M63" t="s">
         <v>105</v>
       </c>
@@ -4172,7 +4166,7 @@
         <v>187</v>
       </c>
       <c r="O63" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="64" spans="1:16">
@@ -4198,19 +4192,19 @@
         <v>70</v>
       </c>
       <c r="H64" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="I64" t="s">
         <v>6</v>
       </c>
       <c r="J64" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="K64" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="L64" s="7" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="M64" t="s">
         <v>105</v>
@@ -4219,7 +4213,7 @@
         <v>187</v>
       </c>
       <c r="O64" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="65" spans="1:16">
@@ -4245,19 +4239,19 @@
         <v>70</v>
       </c>
       <c r="H65" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="I65" t="s">
         <v>6</v>
       </c>
       <c r="J65" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="K65" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="L65" s="7" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="M65" t="s">
         <v>105</v>
@@ -4266,7 +4260,7 @@
         <v>187</v>
       </c>
       <c r="O65" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="66" spans="1:16" ht="30">
@@ -4293,19 +4287,19 @@
         <v>70</v>
       </c>
       <c r="H66" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="I66" t="s">
         <v>6</v>
       </c>
       <c r="J66" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="K66" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="L66" s="7" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="M66" t="s">
         <v>105</v>
@@ -4338,16 +4332,16 @@
         <v>70</v>
       </c>
       <c r="H67" s="16" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="I67" s="16" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="J67" s="16" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="K67" s="16" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="L67" s="17"/>
       <c r="M67" s="16" t="s">
@@ -4381,19 +4375,19 @@
         <v>70</v>
       </c>
       <c r="H68" s="16" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="I68" s="16" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="J68" s="16" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="K68" s="16" t="s">
+        <v>211</v>
+      </c>
+      <c r="L68" s="17" t="s">
         <v>212</v>
-      </c>
-      <c r="L68" s="17" t="s">
-        <v>213</v>
       </c>
       <c r="M68" s="16" t="s">
         <v>105</v>
@@ -4426,19 +4420,19 @@
         <v>70</v>
       </c>
       <c r="H69" s="16" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="I69" s="16" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="J69" s="16" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="K69" s="16" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="L69" s="17" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="M69" s="16" t="s">
         <v>105</v>
@@ -4471,19 +4465,19 @@
         <v>70</v>
       </c>
       <c r="H70" s="16" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="I70" s="16" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="J70" s="16" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="K70" s="16" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="L70" s="17" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="M70" s="16" t="s">
         <v>105</v>
@@ -4516,19 +4510,19 @@
         <v>70</v>
       </c>
       <c r="H71" s="16" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="I71" s="16" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="J71" s="16" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="K71" s="16" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="L71" s="17" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="M71" s="16" t="s">
         <v>105</v>
@@ -4561,19 +4555,19 @@
         <v>70</v>
       </c>
       <c r="H72" s="16" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="I72" s="16" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="J72" s="16" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="K72" s="16" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="L72" s="17" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="M72" s="16" t="s">
         <v>105</v>
@@ -4606,19 +4600,19 @@
         <v>70</v>
       </c>
       <c r="H73" s="16" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="I73" s="16" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="J73" s="16" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="K73" s="16" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="L73" s="17" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="M73" s="16" t="s">
         <v>105</v>
@@ -4650,19 +4644,19 @@
         <v>70</v>
       </c>
       <c r="H74" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="I74" t="s">
         <v>6</v>
       </c>
       <c r="J74" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="K74" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="L74" s="8" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="M74" t="s">
         <v>105</v>
@@ -4671,7 +4665,7 @@
         <v>187</v>
       </c>
       <c r="O74" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="75" spans="1:16">
@@ -4697,19 +4691,19 @@
         <v>70</v>
       </c>
       <c r="H75" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="I75" t="s">
         <v>6</v>
       </c>
       <c r="J75" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="K75" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="L75" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="M75" t="s">
         <v>105</v>
@@ -4718,7 +4712,7 @@
         <v>187</v>
       </c>
       <c r="O75" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="76" spans="1:16" s="9" customFormat="1" ht="30">
@@ -4744,19 +4738,19 @@
         <v>70</v>
       </c>
       <c r="H76" s="9" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="I76" s="9" t="s">
         <v>6</v>
       </c>
       <c r="J76" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="K76" s="9" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="L76" s="8" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="M76" s="9" t="s">
         <v>105</v>
@@ -4765,7 +4759,7 @@
         <v>187</v>
       </c>
       <c r="O76" s="9" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="77" spans="1:16" s="9" customFormat="1">
@@ -4798,10 +4792,10 @@
         <v>6</v>
       </c>
       <c r="J77" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="K77" s="9" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="L77" s="8"/>
       <c r="P77" s="9" t="s">
@@ -4831,19 +4825,19 @@
         <v>70</v>
       </c>
       <c r="H78" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="I78" t="s">
         <v>6</v>
       </c>
       <c r="J78" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="K78" s="9" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="L78" s="7" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="M78" t="s">
         <v>105</v>
@@ -4852,7 +4846,7 @@
         <v>187</v>
       </c>
       <c r="O78" s="9" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="79" spans="1:16">
@@ -4878,19 +4872,19 @@
         <v>70</v>
       </c>
       <c r="H79" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="I79" s="9" t="s">
         <v>6</v>
       </c>
       <c r="J79" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="K79" s="9" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="L79" s="7" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="M79" t="s">
         <v>105</v>
@@ -4899,7 +4893,7 @@
         <v>187</v>
       </c>
       <c r="O79" s="9" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="80" spans="1:16">
@@ -4925,19 +4919,19 @@
         <v>70</v>
       </c>
       <c r="H80" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="I80" s="9" t="s">
         <v>6</v>
       </c>
       <c r="J80" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="K80" s="9" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="L80" s="7" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="M80" t="s">
         <v>105</v>
@@ -4946,7 +4940,7 @@
         <v>187</v>
       </c>
       <c r="O80" s="9" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="81" spans="1:16" s="16" customFormat="1">
@@ -4972,19 +4966,19 @@
         <v>70</v>
       </c>
       <c r="H81" s="16" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="I81" s="16" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="J81" s="16" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="K81" s="16" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="L81" s="17" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="M81" s="16" t="s">
         <v>105</v>
@@ -4993,7 +4987,7 @@
         <v>187</v>
       </c>
       <c r="O81" s="16" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="82" spans="1:16" s="9" customFormat="1">
@@ -5019,16 +5013,16 @@
         <v>70</v>
       </c>
       <c r="H82" s="9" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="I82" s="9" t="s">
         <v>6</v>
       </c>
       <c r="J82" s="9" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="K82" s="9" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="L82" s="8"/>
       <c r="M82" s="9" t="s">
@@ -5038,7 +5032,7 @@
         <v>187</v>
       </c>
       <c r="P82" s="9" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="83" spans="1:16">
@@ -5071,13 +5065,13 @@
         <v>6</v>
       </c>
       <c r="J83" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="K83" s="9" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="L83" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="84" spans="1:16">
@@ -5103,19 +5097,19 @@
         <v>70</v>
       </c>
       <c r="H84" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="I84" s="9" t="s">
         <v>6</v>
       </c>
       <c r="J84" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="K84" s="9" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="L84" s="8" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="M84" t="s">
         <v>105</v>
@@ -5124,7 +5118,7 @@
         <v>187</v>
       </c>
       <c r="O84" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="85" spans="1:16">
@@ -5157,10 +5151,10 @@
         <v>6</v>
       </c>
       <c r="J85" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="K85" s="9" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="86" spans="1:16">
@@ -5186,19 +5180,19 @@
         <v>70</v>
       </c>
       <c r="H86" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="I86" s="9" t="s">
         <v>6</v>
       </c>
       <c r="J86" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="K86" s="9" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="L86" s="7" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="M86" t="s">
         <v>105</v>
@@ -5207,7 +5201,7 @@
         <v>187</v>
       </c>
       <c r="P86" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="87" spans="1:16">
@@ -5240,13 +5234,13 @@
         <v>6</v>
       </c>
       <c r="J87" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="K87" s="9" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="L87" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="88" spans="1:16" ht="30">
@@ -5272,28 +5266,28 @@
         <v>70</v>
       </c>
       <c r="H88" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="I88" s="9" t="s">
         <v>6</v>
       </c>
       <c r="J88" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="K88" s="9" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="L88" s="8" t="s">
+        <v>273</v>
+      </c>
+      <c r="M88" t="s">
+        <v>105</v>
+      </c>
+      <c r="N88" t="s">
+        <v>187</v>
+      </c>
+      <c r="O88" t="s">
         <v>274</v>
-      </c>
-      <c r="M88" t="s">
-        <v>105</v>
-      </c>
-      <c r="N88" t="s">
-        <v>187</v>
-      </c>
-      <c r="O88" t="s">
-        <v>275</v>
       </c>
     </row>
     <row r="89" spans="1:16">
@@ -5326,13 +5320,13 @@
         <v>6</v>
       </c>
       <c r="J89" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="K89" s="9" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="L89" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="90" spans="1:16">
@@ -5359,19 +5353,19 @@
         <v>70</v>
       </c>
       <c r="H90" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="I90" s="9" t="s">
         <v>6</v>
       </c>
       <c r="J90" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="K90" s="12" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="L90" s="8" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="M90" t="s">
         <v>105</v>
@@ -5407,16 +5401,16 @@
         <v>70</v>
       </c>
       <c r="H91" t="s">
+        <v>210</v>
+      </c>
+      <c r="I91" t="s">
+        <v>6</v>
+      </c>
+      <c r="J91" t="s">
+        <v>254</v>
+      </c>
+      <c r="K91" t="s">
         <v>211</v>
-      </c>
-      <c r="I91" t="s">
-        <v>6</v>
-      </c>
-      <c r="J91" t="s">
-        <v>255</v>
-      </c>
-      <c r="K91" t="s">
-        <v>212</v>
       </c>
       <c r="L91" s="8"/>
       <c r="M91" t="s">
@@ -5459,7 +5453,7 @@
         <v>73</v>
       </c>
       <c r="K92" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="93" spans="1:16">
@@ -5486,19 +5480,19 @@
         <v>70</v>
       </c>
       <c r="H93" t="s">
+        <v>210</v>
+      </c>
+      <c r="I93" t="s">
+        <v>6</v>
+      </c>
+      <c r="J93" t="s">
+        <v>254</v>
+      </c>
+      <c r="K93" t="s">
         <v>211</v>
       </c>
-      <c r="I93" t="s">
-        <v>6</v>
-      </c>
-      <c r="J93" t="s">
-        <v>255</v>
-      </c>
-      <c r="K93" t="s">
-        <v>212</v>
-      </c>
       <c r="L93" s="8" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="M93" t="s">
         <v>105</v>
@@ -5512,7 +5506,7 @@
     </row>
     <row r="94" spans="1:16">
       <c r="A94" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B94" t="s">
         <v>11</v>
@@ -5543,7 +5537,7 @@
         <v>73</v>
       </c>
       <c r="K94" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="95" spans="1:16">
@@ -5579,7 +5573,7 @@
         <v>73</v>
       </c>
       <c r="K95" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="96" spans="1:16" ht="30">
@@ -5606,7 +5600,7 @@
         <v>70</v>
       </c>
       <c r="H96" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="I96" t="s">
         <v>6</v>
@@ -5615,10 +5609,10 @@
         <v>73</v>
       </c>
       <c r="K96" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="L96" s="7" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="M96" t="s">
         <v>105</v>
@@ -5651,7 +5645,7 @@
         <v>70</v>
       </c>
       <c r="H97" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="I97" t="s">
         <v>6</v>
@@ -5660,7 +5654,7 @@
         <v>73</v>
       </c>
       <c r="K97" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="M97" t="s">
         <v>105</v>
@@ -5696,7 +5690,7 @@
         <v>70</v>
       </c>
       <c r="H98" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="I98" t="s">
         <v>6</v>
@@ -5705,7 +5699,7 @@
         <v>73</v>
       </c>
       <c r="K98" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="M98" t="s">
         <v>105</v>
@@ -5747,7 +5741,7 @@
         <v>73</v>
       </c>
       <c r="K99" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="M99" t="s">
         <v>105</v>
@@ -5792,10 +5786,10 @@
         <v>73</v>
       </c>
       <c r="K100" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="L100" s="7" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="M100" t="s">
         <v>105</v>
@@ -5837,7 +5831,7 @@
         <v>73</v>
       </c>
       <c r="K101" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="102" spans="1:16">
@@ -5873,10 +5867,10 @@
         <v>73</v>
       </c>
       <c r="K102" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="L102" s="7" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="M102" t="s">
         <v>105</v>
@@ -5918,10 +5912,10 @@
         <v>73</v>
       </c>
       <c r="K103" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="L103" s="7" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="104" spans="1:16">
@@ -5957,7 +5951,7 @@
         <v>73</v>
       </c>
       <c r="K104" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="M104" t="s">
         <v>105</v>
@@ -5999,7 +5993,7 @@
         <v>73</v>
       </c>
       <c r="K105" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="M105" t="s">
         <v>105</v>
@@ -6035,16 +6029,16 @@
         <v>73</v>
       </c>
       <c r="I106" s="16" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="J106" t="s">
         <v>73</v>
       </c>
       <c r="K106" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="L106" s="7" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="M106" t="s">
         <v>105</v>
@@ -6086,7 +6080,7 @@
         <v>73</v>
       </c>
       <c r="K107" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="108" spans="1:16">
@@ -6147,13 +6141,13 @@
         <v>73</v>
       </c>
       <c r="I109" s="16" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="J109" t="s">
         <v>73</v>
       </c>
       <c r="L109" s="7" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="110" spans="1:16">
@@ -6291,7 +6285,7 @@
         <v>73</v>
       </c>
       <c r="L113" s="7" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="114" spans="1:16">
@@ -6327,7 +6321,7 @@
         <v>73</v>
       </c>
       <c r="L114" s="7" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="P114" t="s">
         <v>6</v>
@@ -6399,7 +6393,7 @@
         <v>73</v>
       </c>
       <c r="L116" s="7" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="117" spans="1:16" ht="30">
@@ -6426,16 +6420,16 @@
         <v>70</v>
       </c>
       <c r="H117" t="s">
+        <v>193</v>
+      </c>
+      <c r="I117" s="16" t="s">
+        <v>256</v>
+      </c>
+      <c r="J117" t="s">
         <v>194</v>
       </c>
-      <c r="I117" s="16" t="s">
-        <v>257</v>
-      </c>
-      <c r="J117" t="s">
-        <v>195</v>
-      </c>
       <c r="L117" s="7" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="118" spans="1:16">
@@ -6462,13 +6456,13 @@
         <v>70</v>
       </c>
       <c r="H118" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="I118" s="9" t="s">
         <v>6</v>
       </c>
       <c r="J118" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="119" spans="1:16">
@@ -6495,13 +6489,13 @@
         <v>70</v>
       </c>
       <c r="H119" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="I119" s="9" t="s">
         <v>6</v>
       </c>
       <c r="J119" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="120" spans="1:16">
@@ -6528,13 +6522,13 @@
         <v>70</v>
       </c>
       <c r="H120" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="I120" s="9" t="s">
         <v>6</v>
       </c>
       <c r="L120" s="7" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="121" spans="1:16">
@@ -6561,7 +6555,7 @@
         <v>70</v>
       </c>
       <c r="H121" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="I121" s="9" t="s">
         <v>6</v>
@@ -6594,7 +6588,7 @@
         <v>70</v>
       </c>
       <c r="H122" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="I122" s="9" t="s">
         <v>6</v>
@@ -6624,7 +6618,7 @@
         <v>70</v>
       </c>
       <c r="H123" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="I123" s="9" t="s">
         <v>6</v>
@@ -6654,7 +6648,7 @@
         <v>70</v>
       </c>
       <c r="H124" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="I124" s="9" t="s">
         <v>6</v>
@@ -6682,10 +6676,10 @@
         <v>70</v>
       </c>
       <c r="H125" s="16" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="I125" s="16" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="L125" s="17"/>
       <c r="M125" s="16" t="s">
@@ -6719,7 +6713,7 @@
         <v>70</v>
       </c>
       <c r="H126" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="I126" s="9" t="s">
         <v>6</v>
@@ -6749,7 +6743,7 @@
         <v>70</v>
       </c>
       <c r="H127" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="I127" s="9" t="s">
         <v>6</v>
@@ -6779,7 +6773,7 @@
         <v>70</v>
       </c>
       <c r="H128" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="I128" s="9" t="s">
         <v>6</v>
@@ -6812,7 +6806,7 @@
         <v>70</v>
       </c>
       <c r="H129" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="I129" s="9" t="s">
         <v>6</v>
@@ -6846,7 +6840,7 @@
         <v>189</v>
       </c>
       <c r="I130" s="16" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="J130" s="16" t="s">
         <v>73</v>
@@ -6919,7 +6913,7 @@
         <v>70</v>
       </c>
       <c r="H132" s="9" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="I132" t="s">
         <v>6</v>
@@ -6949,7 +6943,7 @@
         <v>70</v>
       </c>
       <c r="H133" s="9" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="I133" t="s">
         <v>6</v>
@@ -6979,7 +6973,7 @@
         <v>70</v>
       </c>
       <c r="H134" s="9" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="I134" t="s">
         <v>6</v>
@@ -7009,7 +7003,7 @@
         <v>70</v>
       </c>
       <c r="H135" s="9" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="I135" t="s">
         <v>6</v>
@@ -7037,10 +7031,10 @@
         <v>70</v>
       </c>
       <c r="H136" s="16" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="I136" s="16" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="L136" s="17"/>
       <c r="M136" s="16" t="s">
@@ -7074,42 +7068,42 @@
         <v>70</v>
       </c>
       <c r="H137" s="9" t="s">
+        <v>279</v>
+      </c>
+      <c r="I137" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="138" spans="1:16" s="21" customFormat="1" ht="30">
+      <c r="A138" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="B138" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="C138" s="22">
+        <v>28</v>
+      </c>
+      <c r="D138" s="22">
+        <v>26</v>
+      </c>
+      <c r="E138" s="22">
+        <v>2</v>
+      </c>
+      <c r="F138" s="22"/>
+      <c r="G138" s="23" t="s">
+        <v>70</v>
+      </c>
+      <c r="H138" s="21" t="s">
+        <v>279</v>
+      </c>
+      <c r="I138" s="21" t="s">
+        <v>256</v>
+      </c>
+      <c r="L138" s="24" t="s">
         <v>280</v>
       </c>
-      <c r="I137" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="138" spans="1:16" s="16" customFormat="1" ht="30">
-      <c r="A138" s="16" t="s">
-        <v>49</v>
-      </c>
-      <c r="B138" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="C138" s="14">
-        <v>28</v>
-      </c>
-      <c r="D138" s="14">
-        <v>26</v>
-      </c>
-      <c r="E138" s="14">
-        <v>2</v>
-      </c>
-      <c r="F138" s="14"/>
-      <c r="G138" s="24" t="s">
-        <v>70</v>
-      </c>
-      <c r="H138" s="16" t="s">
-        <v>280</v>
-      </c>
-      <c r="I138" s="16" t="s">
-        <v>257</v>
-      </c>
-      <c r="L138" s="17" t="s">
-        <v>281</v>
-      </c>
-      <c r="P138" s="16" t="s">
+      <c r="P138" s="21" t="s">
         <v>6</v>
       </c>
     </row>
@@ -7137,7 +7131,7 @@
         <v>70</v>
       </c>
       <c r="H139" s="9" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="I139" t="s">
         <v>6</v>
@@ -7170,7 +7164,7 @@
         <v>70</v>
       </c>
       <c r="H140" s="9" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="I140" s="9" t="s">
         <v>6</v>
@@ -7200,7 +7194,7 @@
         <v>70</v>
       </c>
       <c r="H141" s="9" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="I141" s="9" t="s">
         <v>6</v>
@@ -7233,7 +7227,7 @@
         <v>70</v>
       </c>
       <c r="H142" s="9" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="I142" s="9" t="s">
         <v>6</v>
@@ -7263,7 +7257,7 @@
         <v>70</v>
       </c>
       <c r="H143" s="9" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="I143" s="9" t="s">
         <v>6</v>
@@ -7299,7 +7293,7 @@
         <v>70</v>
       </c>
       <c r="H144" s="9" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="I144" s="9" t="s">
         <v>6</v>
@@ -7335,7 +7329,7 @@
         <v>70</v>
       </c>
       <c r="H145" s="9" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="I145" s="9" t="s">
         <v>6</v>
@@ -7365,7 +7359,7 @@
         <v>70</v>
       </c>
       <c r="H146" s="9" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="I146" s="9" t="s">
         <v>6</v>
@@ -7398,7 +7392,7 @@
         <v>70</v>
       </c>
       <c r="H147" s="9" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="I147" s="9" t="s">
         <v>6</v>
@@ -7440,7 +7434,7 @@
         <v>73</v>
       </c>
       <c r="L148" s="7" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="P148" t="s">
         <v>6</v>
@@ -7470,7 +7464,7 @@
         <v>70</v>
       </c>
       <c r="H149" s="9" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="I149" t="s">
         <v>6</v>
@@ -7539,7 +7533,7 @@
         <v>70</v>
       </c>
       <c r="H151" s="9" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="I151" t="s">
         <v>6</v>
@@ -7572,7 +7566,7 @@
         <v>70</v>
       </c>
       <c r="H152" s="9" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="I152" t="s">
         <v>6</v>
@@ -7605,7 +7599,7 @@
         <v>70</v>
       </c>
       <c r="H153" s="9" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="I153" t="s">
         <v>6</v>
@@ -7638,7 +7632,7 @@
         <v>70</v>
       </c>
       <c r="H154" s="9" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="I154" t="s">
         <v>6</v>
@@ -7668,13 +7662,13 @@
         <v>70</v>
       </c>
       <c r="H155" s="9" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="I155" t="s">
         <v>6</v>
       </c>
       <c r="L155" s="7" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="P155" t="s">
         <v>6</v>
@@ -7704,45 +7698,46 @@
         <v>70</v>
       </c>
       <c r="H156" s="9" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="I156" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="157" spans="1:16" s="20" customFormat="1">
-      <c r="A157" s="20" t="s">
+    <row r="157" spans="1:16" s="9" customFormat="1">
+      <c r="A157" s="9" t="s">
         <v>175</v>
       </c>
-      <c r="B157" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="C157" s="21">
-        <v>24</v>
-      </c>
-      <c r="D157" s="21">
-        <v>24</v>
-      </c>
-      <c r="E157" s="21">
+      <c r="B157" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C157" s="10">
+        <v>24</v>
+      </c>
+      <c r="D157" s="10">
+        <v>24</v>
+      </c>
+      <c r="E157" s="10">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F157" s="21">
-        <v>0</v>
-      </c>
-      <c r="G157" s="22" t="s">
-        <v>70</v>
-      </c>
-      <c r="H157" s="20" t="s">
-        <v>190</v>
-      </c>
-      <c r="L157" s="23" t="s">
-        <v>283</v>
-      </c>
-      <c r="M157" s="20" t="s">
-        <v>105</v>
-      </c>
-      <c r="N157" s="20" t="s">
+      <c r="F157" s="10">
+        <v>0</v>
+      </c>
+      <c r="G157" s="20" t="s">
+        <v>70</v>
+      </c>
+      <c r="H157" s="9" t="s">
+        <v>278</v>
+      </c>
+      <c r="I157" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="L157" s="8"/>
+      <c r="M157" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="N157" s="9" t="s">
         <v>184</v>
       </c>
     </row>
@@ -7770,7 +7765,7 @@
         <v>70</v>
       </c>
       <c r="H158" s="9" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="I158" t="s">
         <v>6</v>
@@ -7800,7 +7795,7 @@
         <v>70</v>
       </c>
       <c r="H159" s="9" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="I159" t="s">
         <v>6</v>
@@ -7833,10 +7828,10 @@
         <v>70</v>
       </c>
       <c r="H160" s="16" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="I160" s="16" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="L160" s="17"/>
       <c r="M160" s="16" t="s">
@@ -7870,10 +7865,10 @@
         <v>70</v>
       </c>
       <c r="H161" s="16" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="I161" s="16" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="L161" s="17"/>
       <c r="M161" s="16" t="s">
@@ -8048,7 +8043,7 @@
         <v>73</v>
       </c>
       <c r="L166" s="7" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="M166" t="s">
         <v>105</v>

</xml_diff>